<commit_message>
Fix C# Test Generation for Anova test
This involved fixing a bug in the spreadhsheet (df_within was wrong)
and adding some "usings" to the test generation script
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/Anova.xlsx
+++ b/SampleTests/ExcelTests/Anova.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\SampleTests\ExcelTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA575291-574D-4F54-9485-B2950EAC4F74}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7617A041-6382-434B-99C4-F1D987956B0C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="52">
   <si>
     <t>Example from:</t>
   </si>
@@ -142,9 +142,6 @@
     <t>Assert</t>
   </si>
   <si>
-    <t>Returns</t>
-  </si>
-  <si>
     <t>=</t>
   </si>
   <si>
@@ -158,6 +155,27 @@
   </si>
   <si>
     <t>EffectSize</t>
+  </si>
+  <si>
+    <t>PercentagePrecision</t>
+  </si>
+  <si>
+    <t>SS_Between</t>
+  </si>
+  <si>
+    <t>DF_Between</t>
+  </si>
+  <si>
+    <t>MS_Between</t>
+  </si>
+  <si>
+    <t>SS_Within</t>
+  </si>
+  <si>
+    <t>DF_Within</t>
+  </si>
+  <si>
+    <t>MS_Within</t>
   </si>
 </sst>
 </file>
@@ -292,29 +310,7 @@
     <cellStyle name="Accent4" xfId="1" builtinId="41"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -652,8 +648,8 @@
   </sheetPr>
   <dimension ref="A1:AC1021"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -984,7 +980,7 @@
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10">
-        <f>AVERAGE(F$12:F$21)</f>
+        <f t="shared" ref="H12:H21" si="0">AVERAGE(F$12:F$21)</f>
         <v>99.2</v>
       </c>
       <c r="I12" s="10">
@@ -992,19 +988,19 @@
         <v>101.7</v>
       </c>
       <c r="J12" s="10">
-        <f>H12-I12</f>
+        <f t="shared" ref="J12:J21" si="1">H12-I12</f>
         <v>-2.5</v>
       </c>
       <c r="K12" s="10">
-        <f>J12^2</f>
+        <f t="shared" ref="K12:K21" si="2">J12^2</f>
         <v>6.25</v>
       </c>
       <c r="L12" s="10">
-        <f>F12-H12</f>
+        <f t="shared" ref="L12:L21" si="3">F12-H12</f>
         <v>-9.2000000000000028</v>
       </c>
       <c r="M12" s="10">
-        <f>L12^2</f>
+        <f t="shared" ref="M12:M21" si="4">L12^2</f>
         <v>84.640000000000057</v>
       </c>
       <c r="N12" s="10">
@@ -1037,27 +1033,27 @@
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="10">
-        <f>AVERAGE(F$12:F$21)</f>
+        <f t="shared" si="0"/>
         <v>99.2</v>
       </c>
       <c r="I13" s="10">
-        <f t="shared" ref="I13:I21" si="0">AVERAGE(F$12:F$53)</f>
+        <f t="shared" ref="I13:I21" si="5">AVERAGE(F$12:F$53)</f>
         <v>101.7</v>
       </c>
       <c r="J13" s="10">
-        <f>H13-I13</f>
+        <f t="shared" si="1"/>
         <v>-2.5</v>
       </c>
       <c r="K13" s="10">
-        <f>J13^2</f>
+        <f t="shared" si="2"/>
         <v>6.25</v>
       </c>
       <c r="L13" s="10">
-        <f>F13-H13</f>
+        <f t="shared" si="3"/>
         <v>-12.200000000000003</v>
       </c>
       <c r="M13" s="10">
-        <f>L13^2</f>
+        <f t="shared" si="4"/>
         <v>148.84000000000006</v>
       </c>
       <c r="N13" s="10">
@@ -1065,7 +1061,7 @@
         <v>3</v>
       </c>
       <c r="O13" s="10">
-        <f t="shared" ref="O13:O21" si="1">COUNT(F$12:F$53)</f>
+        <f t="shared" ref="O13:O21" si="6">COUNT(F$12:F$53)</f>
         <v>30</v>
       </c>
       <c r="R13" s="10"/>
@@ -1088,27 +1084,27 @@
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="10">
-        <f>AVERAGE(F$12:F$21)</f>
+        <f t="shared" si="0"/>
         <v>99.2</v>
       </c>
       <c r="I14" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>101.7</v>
       </c>
       <c r="J14" s="10">
-        <f>H14-I14</f>
+        <f t="shared" si="1"/>
         <v>-2.5</v>
       </c>
       <c r="K14" s="10">
-        <f>J14^2</f>
+        <f t="shared" si="2"/>
         <v>6.25</v>
       </c>
       <c r="L14" s="10">
-        <f>F14-H14</f>
+        <f t="shared" si="3"/>
         <v>-6.2000000000000028</v>
       </c>
       <c r="M14" s="10">
-        <f>L14^2</f>
+        <f t="shared" si="4"/>
         <v>38.440000000000033</v>
       </c>
       <c r="N14" s="10">
@@ -1116,7 +1112,7 @@
         <v>3</v>
       </c>
       <c r="O14" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="R14" s="10"/>
@@ -1139,27 +1135,27 @@
       </c>
       <c r="G15" s="10"/>
       <c r="H15" s="10">
-        <f>AVERAGE(F$12:F$21)</f>
+        <f t="shared" si="0"/>
         <v>99.2</v>
       </c>
       <c r="I15" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>101.7</v>
       </c>
       <c r="J15" s="10">
-        <f>H15-I15</f>
+        <f t="shared" si="1"/>
         <v>-2.5</v>
       </c>
       <c r="K15" s="10">
-        <f>J15^2</f>
+        <f t="shared" si="2"/>
         <v>6.25</v>
       </c>
       <c r="L15" s="10">
-        <f>F15-H15</f>
+        <f t="shared" si="3"/>
         <v>15.799999999999997</v>
       </c>
       <c r="M15" s="10">
-        <f>L15^2</f>
+        <f t="shared" si="4"/>
         <v>249.6399999999999</v>
       </c>
       <c r="N15" s="10">
@@ -1167,7 +1163,7 @@
         <v>3</v>
       </c>
       <c r="O15" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="R15" s="10"/>
@@ -1190,27 +1186,27 @@
       </c>
       <c r="G16" s="10"/>
       <c r="H16" s="10">
-        <f>AVERAGE(F$12:F$21)</f>
+        <f t="shared" si="0"/>
         <v>99.2</v>
       </c>
       <c r="I16" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>101.7</v>
       </c>
       <c r="J16" s="10">
-        <f>H16-I16</f>
+        <f t="shared" si="1"/>
         <v>-2.5</v>
       </c>
       <c r="K16" s="10">
-        <f>J16^2</f>
+        <f t="shared" si="2"/>
         <v>6.25</v>
       </c>
       <c r="L16" s="10">
-        <f>F16-H16</f>
+        <f t="shared" si="3"/>
         <v>-2.2000000000000028</v>
       </c>
       <c r="M16" s="10">
-        <f>L16^2</f>
+        <f t="shared" si="4"/>
         <v>4.8400000000000123</v>
       </c>
       <c r="N16" s="10">
@@ -1218,7 +1214,7 @@
         <v>3</v>
       </c>
       <c r="O16" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="R16" s="10"/>
@@ -1241,27 +1237,27 @@
       </c>
       <c r="G17" s="10"/>
       <c r="H17" s="10">
-        <f>AVERAGE(F$12:F$21)</f>
+        <f t="shared" si="0"/>
         <v>99.2</v>
       </c>
       <c r="I17" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>101.7</v>
       </c>
       <c r="J17" s="10">
-        <f>H17-I17</f>
+        <f t="shared" si="1"/>
         <v>-2.5</v>
       </c>
       <c r="K17" s="10">
-        <f>J17^2</f>
+        <f t="shared" si="2"/>
         <v>6.25</v>
       </c>
       <c r="L17" s="10">
-        <f>F17-H17</f>
+        <f t="shared" si="3"/>
         <v>-14.200000000000003</v>
       </c>
       <c r="M17" s="10">
-        <f>L17^2</f>
+        <f t="shared" si="4"/>
         <v>201.64000000000007</v>
       </c>
       <c r="N17" s="10">
@@ -1269,7 +1265,7 @@
         <v>3</v>
       </c>
       <c r="O17" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="R17" s="10"/>
@@ -1292,27 +1288,27 @@
       </c>
       <c r="G18" s="10"/>
       <c r="H18" s="10">
-        <f>AVERAGE(F$12:F$21)</f>
+        <f t="shared" si="0"/>
         <v>99.2</v>
       </c>
       <c r="I18" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>101.7</v>
       </c>
       <c r="J18" s="10">
-        <f>H18-I18</f>
+        <f t="shared" si="1"/>
         <v>-2.5</v>
       </c>
       <c r="K18" s="10">
-        <f>J18^2</f>
+        <f t="shared" si="2"/>
         <v>6.25</v>
       </c>
       <c r="L18" s="10">
-        <f>F18-H18</f>
+        <f t="shared" si="3"/>
         <v>2.7999999999999972</v>
       </c>
       <c r="M18" s="10">
-        <f>L18^2</f>
+        <f t="shared" si="4"/>
         <v>7.8399999999999839</v>
       </c>
       <c r="N18" s="10">
@@ -1320,7 +1316,7 @@
         <v>3</v>
       </c>
       <c r="O18" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="R18" s="10"/>
@@ -1343,27 +1339,27 @@
       </c>
       <c r="G19" s="10"/>
       <c r="H19" s="10">
-        <f>AVERAGE(F$12:F$21)</f>
+        <f t="shared" si="0"/>
         <v>99.2</v>
       </c>
       <c r="I19" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>101.7</v>
       </c>
       <c r="J19" s="10">
-        <f>H19-I19</f>
+        <f t="shared" si="1"/>
         <v>-2.5</v>
       </c>
       <c r="K19" s="10">
-        <f>J19^2</f>
+        <f t="shared" si="2"/>
         <v>6.25</v>
       </c>
       <c r="L19" s="10">
-        <f>F19-H19</f>
+        <f t="shared" si="3"/>
         <v>10.799999999999997</v>
       </c>
       <c r="M19" s="10">
-        <f>L19^2</f>
+        <f t="shared" si="4"/>
         <v>116.63999999999994</v>
       </c>
       <c r="N19" s="10">
@@ -1371,7 +1367,7 @@
         <v>3</v>
       </c>
       <c r="O19" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="R19" s="10"/>
@@ -1394,27 +1390,27 @@
       </c>
       <c r="G20" s="10"/>
       <c r="H20" s="10">
-        <f>AVERAGE(F$12:F$21)</f>
+        <f t="shared" si="0"/>
         <v>99.2</v>
       </c>
       <c r="I20" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>101.7</v>
       </c>
       <c r="J20" s="10">
-        <f>H20-I20</f>
+        <f t="shared" si="1"/>
         <v>-2.5</v>
       </c>
       <c r="K20" s="10">
-        <f>J20^2</f>
+        <f t="shared" si="2"/>
         <v>6.25</v>
       </c>
       <c r="L20" s="10">
-        <f>F20-H20</f>
+        <f t="shared" si="3"/>
         <v>11.799999999999997</v>
       </c>
       <c r="M20" s="10">
-        <f>L20^2</f>
+        <f t="shared" si="4"/>
         <v>139.23999999999992</v>
       </c>
       <c r="N20" s="10">
@@ -1422,7 +1418,7 @@
         <v>3</v>
       </c>
       <c r="O20" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="R20" s="10"/>
@@ -1445,27 +1441,27 @@
       </c>
       <c r="G21" s="10"/>
       <c r="H21" s="10">
-        <f>AVERAGE(F$12:F$21)</f>
+        <f t="shared" si="0"/>
         <v>99.2</v>
       </c>
       <c r="I21" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>101.7</v>
       </c>
       <c r="J21" s="10">
-        <f>H21-I21</f>
+        <f t="shared" si="1"/>
         <v>-2.5</v>
       </c>
       <c r="K21" s="10">
-        <f>J21^2</f>
+        <f t="shared" si="2"/>
         <v>6.25</v>
       </c>
       <c r="L21" s="10">
-        <f>F21-H21</f>
+        <f t="shared" si="3"/>
         <v>2.7999999999999972</v>
       </c>
       <c r="M21" s="10">
-        <f>L21^2</f>
+        <f t="shared" si="4"/>
         <v>7.8399999999999839</v>
       </c>
       <c r="N21" s="10">
@@ -1473,7 +1469,7 @@
         <v>3</v>
       </c>
       <c r="O21" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="R21" s="10"/>
@@ -1679,7 +1675,7 @@
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="10">
-        <f>AVERAGE(F$28:F$37)</f>
+        <f t="shared" ref="H28:H37" si="7">AVERAGE(F$28:F$37)</f>
         <v>112.6</v>
       </c>
       <c r="I28" s="10">
@@ -1687,19 +1683,19 @@
         <v>101.7</v>
       </c>
       <c r="J28" s="10">
-        <f>H28-I28</f>
+        <f t="shared" ref="J28:J37" si="8">H28-I28</f>
         <v>10.899999999999991</v>
       </c>
       <c r="K28" s="10">
-        <f>J28^2</f>
+        <f t="shared" ref="K28:K37" si="9">J28^2</f>
         <v>118.80999999999982</v>
       </c>
       <c r="L28" s="10">
-        <f>F28-H28</f>
+        <f t="shared" ref="L28:L37" si="10">F28-H28</f>
         <v>22.400000000000006</v>
       </c>
       <c r="M28" s="10">
-        <f>L28^2</f>
+        <f t="shared" ref="M28:M37" si="11">L28^2</f>
         <v>501.76000000000028</v>
       </c>
       <c r="N28" s="10">
@@ -1707,7 +1703,7 @@
         <v>3</v>
       </c>
       <c r="O28" s="10">
-        <f t="shared" ref="O28:O37" si="2">COUNT(F$12:F$53)</f>
+        <f t="shared" ref="O28:O37" si="12">COUNT(F$12:F$53)</f>
         <v>30</v>
       </c>
       <c r="P28" s="10"/>
@@ -1732,27 +1728,27 @@
       </c>
       <c r="G29" s="10"/>
       <c r="H29" s="10">
-        <f>AVERAGE(F$28:F$37)</f>
+        <f t="shared" si="7"/>
         <v>112.6</v>
       </c>
       <c r="I29" s="10">
-        <f t="shared" ref="I29:I37" si="3">AVERAGE(F$12:F$53)</f>
+        <f t="shared" ref="I29:I37" si="13">AVERAGE(F$12:F$53)</f>
         <v>101.7</v>
       </c>
       <c r="J29" s="10">
-        <f>H29-I29</f>
+        <f t="shared" si="8"/>
         <v>10.899999999999991</v>
       </c>
       <c r="K29" s="10">
-        <f>J29^2</f>
+        <f t="shared" si="9"/>
         <v>118.80999999999982</v>
       </c>
       <c r="L29" s="10">
-        <f>F29-H29</f>
+        <f t="shared" si="10"/>
         <v>12.400000000000006</v>
       </c>
       <c r="M29" s="10">
-        <f>L29^2</f>
+        <f t="shared" si="11"/>
         <v>153.76000000000013</v>
       </c>
       <c r="N29" s="10">
@@ -1760,7 +1756,7 @@
         <v>3</v>
       </c>
       <c r="O29" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="12"/>
         <v>30</v>
       </c>
       <c r="P29" s="10"/>
@@ -1785,27 +1781,27 @@
       </c>
       <c r="G30" s="10"/>
       <c r="H30" s="10">
-        <f>AVERAGE(F$28:F$37)</f>
+        <f t="shared" si="7"/>
         <v>112.6</v>
       </c>
       <c r="I30" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>101.7</v>
       </c>
       <c r="J30" s="10">
-        <f>H30-I30</f>
+        <f t="shared" si="8"/>
         <v>10.899999999999991</v>
       </c>
       <c r="K30" s="10">
-        <f>J30^2</f>
+        <f t="shared" si="9"/>
         <v>118.80999999999982</v>
       </c>
       <c r="L30" s="10">
-        <f>F30-H30</f>
+        <f t="shared" si="10"/>
         <v>-5.5999999999999943</v>
       </c>
       <c r="M30" s="10">
-        <f>L30^2</f>
+        <f t="shared" si="11"/>
         <v>31.359999999999935</v>
       </c>
       <c r="N30" s="10">
@@ -1813,7 +1809,7 @@
         <v>3</v>
       </c>
       <c r="O30" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="12"/>
         <v>30</v>
       </c>
       <c r="P30" s="10"/>
@@ -1838,27 +1834,27 @@
       </c>
       <c r="G31" s="10"/>
       <c r="H31" s="10">
-        <f>AVERAGE(F$28:F$37)</f>
+        <f t="shared" si="7"/>
         <v>112.6</v>
       </c>
       <c r="I31" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>101.7</v>
       </c>
       <c r="J31" s="10">
-        <f>H31-I31</f>
+        <f t="shared" si="8"/>
         <v>10.899999999999991</v>
       </c>
       <c r="K31" s="10">
-        <f>J31^2</f>
+        <f t="shared" si="9"/>
         <v>118.80999999999982</v>
       </c>
       <c r="L31" s="10">
-        <f>F31-H31</f>
+        <f t="shared" si="10"/>
         <v>-16.599999999999994</v>
       </c>
       <c r="M31" s="10">
-        <f>L31^2</f>
+        <f t="shared" si="11"/>
         <v>275.55999999999983</v>
       </c>
       <c r="N31" s="10">
@@ -1866,7 +1862,7 @@
         <v>3</v>
       </c>
       <c r="O31" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="12"/>
         <v>30</v>
       </c>
       <c r="P31" s="10"/>
@@ -1891,27 +1887,27 @@
       </c>
       <c r="G32" s="10"/>
       <c r="H32" s="10">
-        <f>AVERAGE(F$28:F$37)</f>
+        <f t="shared" si="7"/>
         <v>112.6</v>
       </c>
       <c r="I32" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>101.7</v>
       </c>
       <c r="J32" s="10">
-        <f>H32-I32</f>
+        <f t="shared" si="8"/>
         <v>10.899999999999991</v>
       </c>
       <c r="K32" s="10">
-        <f>J32^2</f>
+        <f t="shared" si="9"/>
         <v>118.80999999999982</v>
       </c>
       <c r="L32" s="10">
-        <f>F32-H32</f>
+        <f t="shared" si="10"/>
         <v>1.4000000000000057</v>
       </c>
       <c r="M32" s="10">
-        <f>L32^2</f>
+        <f t="shared" si="11"/>
         <v>1.960000000000016</v>
       </c>
       <c r="N32" s="10">
@@ -1919,7 +1915,7 @@
         <v>3</v>
       </c>
       <c r="O32" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="12"/>
         <v>30</v>
       </c>
       <c r="P32" s="10"/>
@@ -1944,27 +1940,27 @@
       </c>
       <c r="G33" s="10"/>
       <c r="H33" s="10">
-        <f>AVERAGE(F$28:F$37)</f>
+        <f t="shared" si="7"/>
         <v>112.6</v>
       </c>
       <c r="I33" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>101.7</v>
       </c>
       <c r="J33" s="10">
-        <f>H33-I33</f>
+        <f t="shared" si="8"/>
         <v>10.899999999999991</v>
       </c>
       <c r="K33" s="10">
-        <f>J33^2</f>
+        <f t="shared" si="9"/>
         <v>118.80999999999982</v>
       </c>
       <c r="L33" s="10">
-        <f>F33-H33</f>
+        <f t="shared" si="10"/>
         <v>12.400000000000006</v>
       </c>
       <c r="M33" s="10">
-        <f>L33^2</f>
+        <f t="shared" si="11"/>
         <v>153.76000000000013</v>
       </c>
       <c r="N33" s="10">
@@ -1972,7 +1968,7 @@
         <v>3</v>
       </c>
       <c r="O33" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="12"/>
         <v>30</v>
       </c>
       <c r="P33" s="10"/>
@@ -1997,27 +1993,27 @@
       </c>
       <c r="G34" s="10"/>
       <c r="H34" s="10">
-        <f>AVERAGE(F$28:F$37)</f>
+        <f t="shared" si="7"/>
         <v>112.6</v>
       </c>
       <c r="I34" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>101.7</v>
       </c>
       <c r="J34" s="10">
-        <f>H34-I34</f>
+        <f t="shared" si="8"/>
         <v>10.899999999999991</v>
       </c>
       <c r="K34" s="10">
-        <f>J34^2</f>
+        <f t="shared" si="9"/>
         <v>118.80999999999982</v>
       </c>
       <c r="L34" s="10">
-        <f>F34-H34</f>
+        <f t="shared" si="10"/>
         <v>-18.599999999999994</v>
       </c>
       <c r="M34" s="10">
-        <f>L34^2</f>
+        <f t="shared" si="11"/>
         <v>345.95999999999981</v>
       </c>
       <c r="N34" s="10">
@@ -2025,7 +2021,7 @@
         <v>3</v>
       </c>
       <c r="O34" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="12"/>
         <v>30</v>
       </c>
       <c r="P34" s="10"/>
@@ -2050,27 +2046,27 @@
       </c>
       <c r="G35" s="10"/>
       <c r="H35" s="10">
-        <f>AVERAGE(F$28:F$37)</f>
+        <f t="shared" si="7"/>
         <v>112.6</v>
       </c>
       <c r="I35" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>101.7</v>
       </c>
       <c r="J35" s="10">
-        <f>H35-I35</f>
+        <f t="shared" si="8"/>
         <v>10.899999999999991</v>
       </c>
       <c r="K35" s="10">
-        <f>J35^2</f>
+        <f t="shared" si="9"/>
         <v>118.80999999999982</v>
       </c>
       <c r="L35" s="10">
-        <f>F35-H35</f>
+        <f t="shared" si="10"/>
         <v>10.400000000000006</v>
       </c>
       <c r="M35" s="10">
-        <f>L35^2</f>
+        <f t="shared" si="11"/>
         <v>108.16000000000012</v>
       </c>
       <c r="N35" s="10">
@@ -2078,7 +2074,7 @@
         <v>3</v>
       </c>
       <c r="O35" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="12"/>
         <v>30</v>
       </c>
       <c r="P35" s="10"/>
@@ -2103,27 +2099,27 @@
       </c>
       <c r="G36" s="10"/>
       <c r="H36" s="10">
-        <f>AVERAGE(F$28:F$37)</f>
+        <f t="shared" si="7"/>
         <v>112.6</v>
       </c>
       <c r="I36" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>101.7</v>
       </c>
       <c r="J36" s="10">
-        <f>H36-I36</f>
+        <f t="shared" si="8"/>
         <v>10.899999999999991</v>
       </c>
       <c r="K36" s="10">
-        <f>J36^2</f>
+        <f t="shared" si="9"/>
         <v>118.80999999999982</v>
       </c>
       <c r="L36" s="10">
-        <f>F36-H36</f>
+        <f t="shared" si="10"/>
         <v>-1.5999999999999943</v>
       </c>
       <c r="M36" s="10">
-        <f>L36^2</f>
+        <f t="shared" si="11"/>
         <v>2.5599999999999818</v>
       </c>
       <c r="N36" s="10">
@@ -2131,7 +2127,7 @@
         <v>3</v>
       </c>
       <c r="O36" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="12"/>
         <v>30</v>
       </c>
       <c r="P36" s="10"/>
@@ -2156,27 +2152,27 @@
       </c>
       <c r="G37" s="10"/>
       <c r="H37" s="10">
-        <f>AVERAGE(F$28:F$37)</f>
+        <f t="shared" si="7"/>
         <v>112.6</v>
       </c>
       <c r="I37" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>101.7</v>
       </c>
       <c r="J37" s="10">
-        <f>H37-I37</f>
+        <f t="shared" si="8"/>
         <v>10.899999999999991</v>
       </c>
       <c r="K37" s="10">
-        <f>J37^2</f>
+        <f t="shared" si="9"/>
         <v>118.80999999999982</v>
       </c>
       <c r="L37" s="10">
-        <f>F37-H37</f>
+        <f t="shared" si="10"/>
         <v>-16.599999999999994</v>
       </c>
       <c r="M37" s="10">
-        <f>L37^2</f>
+        <f t="shared" si="11"/>
         <v>275.55999999999983</v>
       </c>
       <c r="N37" s="10">
@@ -2184,7 +2180,7 @@
         <v>3</v>
       </c>
       <c r="O37" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="12"/>
         <v>30</v>
       </c>
       <c r="P37" s="10"/>
@@ -2392,7 +2388,7 @@
       </c>
       <c r="G44" s="10"/>
       <c r="H44" s="10">
-        <f>AVERAGE(F$44:F$53)</f>
+        <f t="shared" ref="H44:H53" si="14">AVERAGE(F$44:F$53)</f>
         <v>93.3</v>
       </c>
       <c r="I44" s="10">
@@ -2400,19 +2396,19 @@
         <v>101.7</v>
       </c>
       <c r="J44" s="10">
-        <f>H44-I44</f>
+        <f t="shared" ref="J44:J53" si="15">H44-I44</f>
         <v>-8.4000000000000057</v>
       </c>
       <c r="K44" s="10">
-        <f>J44^2</f>
+        <f t="shared" ref="K44:K53" si="16">J44^2</f>
         <v>70.560000000000102</v>
       </c>
       <c r="L44" s="10">
-        <f>F44-H44</f>
+        <f t="shared" ref="L44:L53" si="17">F44-H44</f>
         <v>-0.29999999999999716</v>
       </c>
       <c r="M44" s="10">
-        <f>L44^2</f>
+        <f t="shared" ref="M44:M53" si="18">L44^2</f>
         <v>8.999999999999829E-2</v>
       </c>
       <c r="N44" s="10">
@@ -2420,7 +2416,7 @@
         <v>3</v>
       </c>
       <c r="O44" s="10">
-        <f t="shared" ref="O44:O54" si="4">COUNT(F$12:F$53)</f>
+        <f t="shared" ref="O44:O53" si="19">COUNT(F$12:F$53)</f>
         <v>30</v>
       </c>
       <c r="P44" s="10"/>
@@ -2445,27 +2441,27 @@
       </c>
       <c r="G45" s="10"/>
       <c r="H45" s="10">
-        <f>AVERAGE(F$44:F$53)</f>
+        <f t="shared" si="14"/>
         <v>93.3</v>
       </c>
       <c r="I45" s="10">
-        <f t="shared" ref="I45:I53" si="5">AVERAGE(F$12:F$53)</f>
+        <f t="shared" ref="I45:I53" si="20">AVERAGE(F$12:F$53)</f>
         <v>101.7</v>
       </c>
       <c r="J45" s="10">
-        <f>H45-I45</f>
+        <f t="shared" si="15"/>
         <v>-8.4000000000000057</v>
       </c>
       <c r="K45" s="10">
-        <f>J45^2</f>
+        <f t="shared" si="16"/>
         <v>70.560000000000102</v>
       </c>
       <c r="L45" s="10">
-        <f>F45-H45</f>
+        <f t="shared" si="17"/>
         <v>7.7000000000000028</v>
       </c>
       <c r="M45" s="10">
-        <f>L45^2</f>
+        <f t="shared" si="18"/>
         <v>59.290000000000042</v>
       </c>
       <c r="N45" s="10">
@@ -2473,7 +2469,7 @@
         <v>3</v>
       </c>
       <c r="O45" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>30</v>
       </c>
       <c r="P45" s="10"/>
@@ -2498,27 +2494,27 @@
       </c>
       <c r="G46" s="10"/>
       <c r="H46" s="10">
-        <f>AVERAGE(F$44:F$53)</f>
+        <f t="shared" si="14"/>
         <v>93.3</v>
       </c>
       <c r="I46" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="20"/>
         <v>101.7</v>
       </c>
       <c r="J46" s="10">
-        <f>H46-I46</f>
+        <f t="shared" si="15"/>
         <v>-8.4000000000000057</v>
       </c>
       <c r="K46" s="10">
-        <f>J46^2</f>
+        <f t="shared" si="16"/>
         <v>70.560000000000102</v>
       </c>
       <c r="L46" s="10">
-        <f>F46-H46</f>
+        <f t="shared" si="17"/>
         <v>-19.299999999999997</v>
       </c>
       <c r="M46" s="10">
-        <f>L46^2</f>
+        <f t="shared" si="18"/>
         <v>372.4899999999999</v>
       </c>
       <c r="N46" s="10">
@@ -2526,7 +2522,7 @@
         <v>3</v>
       </c>
       <c r="O46" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>30</v>
       </c>
       <c r="P46" s="10"/>
@@ -2551,27 +2547,27 @@
       </c>
       <c r="G47" s="10"/>
       <c r="H47" s="10">
-        <f>AVERAGE(F$44:F$53)</f>
+        <f t="shared" si="14"/>
         <v>93.3</v>
       </c>
       <c r="I47" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="20"/>
         <v>101.7</v>
       </c>
       <c r="J47" s="10">
-        <f>H47-I47</f>
+        <f t="shared" si="15"/>
         <v>-8.4000000000000057</v>
       </c>
       <c r="K47" s="10">
-        <f>J47^2</f>
+        <f t="shared" si="16"/>
         <v>70.560000000000102</v>
       </c>
       <c r="L47" s="10">
-        <f>F47-H47</f>
+        <f t="shared" si="17"/>
         <v>-6.2999999999999972</v>
       </c>
       <c r="M47" s="10">
-        <f>L47^2</f>
+        <f t="shared" si="18"/>
         <v>39.689999999999962</v>
       </c>
       <c r="N47" s="10">
@@ -2579,7 +2575,7 @@
         <v>3</v>
       </c>
       <c r="O47" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>30</v>
       </c>
       <c r="P47" s="10"/>
@@ -2604,27 +2600,27 @@
       </c>
       <c r="G48" s="10"/>
       <c r="H48" s="10">
-        <f>AVERAGE(F$44:F$53)</f>
+        <f t="shared" si="14"/>
         <v>93.3</v>
       </c>
       <c r="I48" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="20"/>
         <v>101.7</v>
       </c>
       <c r="J48" s="10">
-        <f>H48-I48</f>
+        <f t="shared" si="15"/>
         <v>-8.4000000000000057</v>
       </c>
       <c r="K48" s="10">
-        <f>J48^2</f>
+        <f t="shared" si="16"/>
         <v>70.560000000000102</v>
       </c>
       <c r="L48" s="10">
-        <f>F48-H48</f>
+        <f t="shared" si="17"/>
         <v>-17.299999999999997</v>
       </c>
       <c r="M48" s="10">
-        <f>L48^2</f>
+        <f t="shared" si="18"/>
         <v>299.28999999999991</v>
       </c>
       <c r="N48" s="10">
@@ -2632,7 +2628,7 @@
         <v>3</v>
       </c>
       <c r="O48" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>30</v>
       </c>
       <c r="P48" s="10"/>
@@ -2657,27 +2653,27 @@
       </c>
       <c r="G49" s="10"/>
       <c r="H49" s="10">
-        <f>AVERAGE(F$44:F$53)</f>
+        <f t="shared" si="14"/>
         <v>93.3</v>
       </c>
       <c r="I49" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="20"/>
         <v>101.7</v>
       </c>
       <c r="J49" s="10">
-        <f>H49-I49</f>
+        <f t="shared" si="15"/>
         <v>-8.4000000000000057</v>
       </c>
       <c r="K49" s="10">
-        <f>J49^2</f>
+        <f t="shared" si="16"/>
         <v>70.560000000000102</v>
       </c>
       <c r="L49" s="10">
-        <f>F49-H49</f>
+        <f t="shared" si="17"/>
         <v>-6.2999999999999972</v>
       </c>
       <c r="M49" s="10">
-        <f>L49^2</f>
+        <f t="shared" si="18"/>
         <v>39.689999999999962</v>
       </c>
       <c r="N49" s="10">
@@ -2685,7 +2681,7 @@
         <v>3</v>
       </c>
       <c r="O49" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>30</v>
       </c>
       <c r="P49" s="10"/>
@@ -2710,27 +2706,27 @@
       </c>
       <c r="G50" s="10"/>
       <c r="H50" s="10">
-        <f>AVERAGE(F$44:F$53)</f>
+        <f t="shared" si="14"/>
         <v>93.3</v>
       </c>
       <c r="I50" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="20"/>
         <v>101.7</v>
       </c>
       <c r="J50" s="10">
-        <f>H50-I50</f>
+        <f t="shared" si="15"/>
         <v>-8.4000000000000057</v>
       </c>
       <c r="K50" s="10">
-        <f>J50^2</f>
+        <f t="shared" si="16"/>
         <v>70.560000000000102</v>
       </c>
       <c r="L50" s="10">
-        <f>F50-H50</f>
+        <f t="shared" si="17"/>
         <v>4.7000000000000028</v>
       </c>
       <c r="M50" s="10">
-        <f>L50^2</f>
+        <f t="shared" si="18"/>
         <v>22.090000000000028</v>
       </c>
       <c r="N50" s="10">
@@ -2738,7 +2734,7 @@
         <v>3</v>
       </c>
       <c r="O50" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>30</v>
       </c>
       <c r="P50" s="10"/>
@@ -2763,27 +2759,27 @@
       </c>
       <c r="G51" s="10"/>
       <c r="H51" s="10">
-        <f>AVERAGE(F$44:F$53)</f>
+        <f t="shared" si="14"/>
         <v>93.3</v>
       </c>
       <c r="I51" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="20"/>
         <v>101.7</v>
       </c>
       <c r="J51" s="10">
-        <f>H51-I51</f>
+        <f t="shared" si="15"/>
         <v>-8.4000000000000057</v>
       </c>
       <c r="K51" s="10">
-        <f>J51^2</f>
+        <f t="shared" si="16"/>
         <v>70.560000000000102</v>
       </c>
       <c r="L51" s="10">
-        <f>F51-H51</f>
+        <f t="shared" si="17"/>
         <v>14.700000000000003</v>
       </c>
       <c r="M51" s="10">
-        <f>L51^2</f>
+        <f t="shared" si="18"/>
         <v>216.09000000000009</v>
       </c>
       <c r="N51" s="10">
@@ -2791,7 +2787,7 @@
         <v>3</v>
       </c>
       <c r="O51" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>30</v>
       </c>
       <c r="P51" s="10"/>
@@ -2816,27 +2812,27 @@
       </c>
       <c r="G52" s="10"/>
       <c r="H52" s="10">
-        <f>AVERAGE(F$44:F$53)</f>
+        <f t="shared" si="14"/>
         <v>93.3</v>
       </c>
       <c r="I52" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="20"/>
         <v>101.7</v>
       </c>
       <c r="J52" s="10">
-        <f>H52-I52</f>
+        <f t="shared" si="15"/>
         <v>-8.4000000000000057</v>
       </c>
       <c r="K52" s="10">
-        <f>J52^2</f>
+        <f t="shared" si="16"/>
         <v>70.560000000000102</v>
       </c>
       <c r="L52" s="10">
-        <f>F52-H52</f>
+        <f t="shared" si="17"/>
         <v>19.700000000000003</v>
       </c>
       <c r="M52" s="10">
-        <f>L52^2</f>
+        <f t="shared" si="18"/>
         <v>388.09000000000009</v>
       </c>
       <c r="N52" s="10">
@@ -2844,7 +2840,7 @@
         <v>3</v>
       </c>
       <c r="O52" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>30</v>
       </c>
       <c r="P52" s="10"/>
@@ -2869,27 +2865,27 @@
       </c>
       <c r="G53" s="10"/>
       <c r="H53" s="10">
-        <f>AVERAGE(F$44:F$53)</f>
+        <f t="shared" si="14"/>
         <v>93.3</v>
       </c>
       <c r="I53" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="20"/>
         <v>101.7</v>
       </c>
       <c r="J53" s="10">
-        <f>H53-I53</f>
+        <f t="shared" si="15"/>
         <v>-8.4000000000000057</v>
       </c>
       <c r="K53" s="10">
-        <f>J53^2</f>
+        <f t="shared" si="16"/>
         <v>70.560000000000102</v>
       </c>
       <c r="L53" s="10">
-        <f>F53-H53</f>
+        <f t="shared" si="17"/>
         <v>2.7000000000000028</v>
       </c>
       <c r="M53" s="10">
-        <f>L53^2</f>
+        <f t="shared" si="18"/>
         <v>7.2900000000000151</v>
       </c>
       <c r="N53" s="10">
@@ -2897,7 +2893,7 @@
         <v>3</v>
       </c>
       <c r="O53" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="19"/>
         <v>30</v>
       </c>
       <c r="P53" s="10"/>
@@ -2920,7 +2916,7 @@
         <v>38</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C54" s="11"/>
       <c r="E54" s="11"/>
@@ -2942,8 +2938,8 @@
         <v>3</v>
       </c>
       <c r="O54" s="10">
-        <f ca="1">AVERAGE(12:53)</f>
-        <v>60.715925925925923</v>
+        <f>AVERAGE(O12:O53)</f>
+        <v>30</v>
       </c>
       <c r="P54" s="10"/>
       <c r="Q54" s="10"/>
@@ -3027,19 +3023,17 @@
     <row r="57" spans="1:29" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" s="11"/>
       <c r="B57" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D57" s="11"/>
       <c r="E57" s="11"/>
       <c r="F57" s="10"/>
-      <c r="G57" s="10" t="s">
+      <c r="I57" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H57" s="10"/>
-      <c r="I57" s="10"/>
       <c r="J57" s="10"/>
       <c r="K57" s="10"/>
       <c r="L57" s="10"/>
@@ -3065,25 +3059,28 @@
       <c r="A58" s="11"/>
       <c r="B58" s="11"/>
       <c r="C58" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D58" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E58" s="13">
+        <f>J58</f>
+        <v>1956.1999999999998</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G58">
+        <v>1E-3</v>
+      </c>
+      <c r="I58" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D58" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E58" s="13">
-        <f>H58</f>
-        <v>1956.1999999999998</v>
-      </c>
-      <c r="F58" s="10"/>
-      <c r="G58" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H58" s="10">
+      <c r="J58" s="10">
         <f>K54</f>
         <v>1956.1999999999998</v>
       </c>
-      <c r="I58" s="10"/>
-      <c r="J58" s="10"/>
       <c r="K58" s="10"/>
       <c r="L58" s="10"/>
       <c r="M58" s="10"/>
@@ -3108,25 +3105,28 @@
       <c r="A59" s="11"/>
       <c r="B59" s="11"/>
       <c r="C59" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D59" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E59" s="13">
+        <f ca="1">J59</f>
+        <v>2</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G59">
+        <v>1E-3</v>
+      </c>
+      <c r="I59" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D59" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E59" s="13">
-        <f t="shared" ref="E59:E66" ca="1" si="6">H59</f>
-        <v>2</v>
-      </c>
-      <c r="F59" s="10"/>
-      <c r="G59" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H59" s="10">
+      <c r="J59" s="10">
         <f ca="1">N54-1</f>
         <v>2</v>
       </c>
-      <c r="I59" s="10"/>
-      <c r="J59" s="10"/>
       <c r="K59" s="10"/>
       <c r="L59" s="10"/>
       <c r="M59" s="10"/>
@@ -3150,25 +3150,28 @@
     <row r="60" spans="1:29" ht="18" x14ac:dyDescent="0.25">
       <c r="B60" s="4"/>
       <c r="C60" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D60" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E60" s="13">
+        <f ca="1">J60</f>
+        <v>978.09999999999991</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G60">
+        <v>1E-3</v>
+      </c>
+      <c r="I60" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D60" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E60" s="13">
-        <f t="shared" ca="1" si="6"/>
+      <c r="J60" s="10">
+        <f ca="1">J58/J59</f>
         <v>978.09999999999991</v>
       </c>
-      <c r="F60" s="4"/>
-      <c r="G60" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H60" s="10">
-        <f ca="1">H58/H59</f>
-        <v>978.09999999999991</v>
-      </c>
-      <c r="I60" s="4"/>
-      <c r="J60" s="4"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
@@ -3192,25 +3195,28 @@
     <row r="61" spans="1:29" ht="18" x14ac:dyDescent="0.25">
       <c r="B61" s="4"/>
       <c r="C61" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D61" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E61" s="13">
+        <f>J61</f>
+        <v>4294.1000000000004</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G61">
+        <v>1E-3</v>
+      </c>
+      <c r="I61" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D61" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E61" s="13">
-        <f t="shared" si="6"/>
-        <v>4294.1000000000004</v>
-      </c>
-      <c r="F61" s="4"/>
-      <c r="G61" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H61" s="10">
+      <c r="J61" s="10">
         <f>M54</f>
         <v>4294.1000000000004</v>
       </c>
-      <c r="I61" s="4"/>
-      <c r="J61" s="4"/>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
@@ -3234,25 +3240,28 @@
     <row r="62" spans="1:29" ht="18" x14ac:dyDescent="0.25">
       <c r="B62" s="4"/>
       <c r="C62" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E62" s="13">
+        <f ca="1">J62</f>
+        <v>27</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G62">
+        <v>1E-3</v>
+      </c>
+      <c r="I62" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D62" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E62" s="13">
-        <f t="shared" ca="1" si="6"/>
-        <v>57.715925925925923</v>
-      </c>
-      <c r="F62" s="4"/>
-      <c r="G62" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H62" s="10">
+      <c r="J62" s="10">
         <f ca="1">O54-N54</f>
-        <v>57.715925925925923</v>
-      </c>
-      <c r="I62" s="4"/>
-      <c r="J62" s="4"/>
+        <v>27</v>
+      </c>
       <c r="K62" s="4"/>
       <c r="L62" s="4"/>
       <c r="M62" s="4"/>
@@ -3276,25 +3285,28 @@
     <row r="63" spans="1:29" ht="18" x14ac:dyDescent="0.25">
       <c r="B63" s="4"/>
       <c r="C63" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D63" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E63" s="13">
+        <f ca="1">J63</f>
+        <v>159.04074074074074</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G63">
+        <v>1E-3</v>
+      </c>
+      <c r="I63" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D63" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E63" s="13">
-        <f t="shared" ca="1" si="6"/>
-        <v>74.400608343547276</v>
-      </c>
-      <c r="F63" s="4"/>
-      <c r="G63" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H63" s="10">
-        <f ca="1">H61/H62</f>
-        <v>74.400608343547276</v>
-      </c>
-      <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
+      <c r="J63" s="10">
+        <f ca="1">J61/J62</f>
+        <v>159.04074074074074</v>
+      </c>
       <c r="K63" s="4"/>
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
@@ -3321,22 +3333,25 @@
         <v>18</v>
       </c>
       <c r="D64" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E64" s="13">
-        <f t="shared" ca="1" si="6"/>
-        <v>13.146397882710726</v>
-      </c>
-      <c r="F64" s="4"/>
-      <c r="G64" s="10" t="s">
+        <f ca="1">J64</f>
+        <v>6.1499965068349587</v>
+      </c>
+      <c r="F64" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G64">
+        <v>1E-3</v>
+      </c>
+      <c r="I64" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H64" s="10">
-        <f ca="1">H60/H63</f>
-        <v>13.146397882710726</v>
-      </c>
-      <c r="I64" s="4"/>
-      <c r="J64" s="4"/>
+      <c r="J64" s="10">
+        <f ca="1">J60/J63</f>
+        <v>6.1499965068349587</v>
+      </c>
       <c r="K64" s="4"/>
       <c r="L64" s="4"/>
       <c r="M64" s="4"/>
@@ -3360,25 +3375,28 @@
     <row r="65" spans="2:29" ht="18" x14ac:dyDescent="0.25">
       <c r="B65" s="4"/>
       <c r="C65" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E65" s="13">
-        <f t="shared" ca="1" si="6"/>
-        <v>2.0189304431174777E-5</v>
-      </c>
-      <c r="F65" s="4"/>
-      <c r="G65" s="10" t="s">
+        <f ca="1">J65</f>
+        <v>6.2966916787415188E-3</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G65">
+        <v>1E-3</v>
+      </c>
+      <c r="I65" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H65" s="10">
-        <f ca="1">FDIST(H64,H59,H62)</f>
-        <v>2.0189304431174777E-5</v>
-      </c>
-      <c r="I65" s="4"/>
-      <c r="J65" s="4"/>
+      <c r="J65" s="10">
+        <f ca="1">FDIST(J64,J59,J62)</f>
+        <v>6.2966916787415188E-3</v>
+      </c>
       <c r="K65" s="4"/>
       <c r="L65" s="4"/>
       <c r="M65" s="4"/>
@@ -3402,25 +3420,28 @@
     <row r="66" spans="2:29" ht="18" x14ac:dyDescent="0.25">
       <c r="B66" s="4"/>
       <c r="C66" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D66" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E66" s="13">
+        <f>J66</f>
+        <v>0.31297697710509892</v>
+      </c>
+      <c r="F66" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D66" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E66" s="13">
-        <f t="shared" si="6"/>
+      <c r="G66">
+        <v>1E-3</v>
+      </c>
+      <c r="I66" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J66" s="10">
+        <f>J58/(J58+J61)</f>
         <v>0.31297697710509892</v>
       </c>
-      <c r="F66" s="4"/>
-      <c r="G66" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H66" s="10">
-        <f>H58/(H58+H61)</f>
-        <v>0.31297697710509892</v>
-      </c>
-      <c r="I66" s="4"/>
-      <c r="J66" s="4"/>
       <c r="K66" s="4"/>
       <c r="L66" s="4"/>
       <c r="M66" s="4"/>
@@ -32092,13 +32113,13 @@
       <c r="AC1021" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD4 A67:XFD1048576 P6:XFD8 A54:C57 E5:XFD5 S9:XFD59 A5:A53 A58:B66 F60:XFD66">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+  <conditionalFormatting sqref="A1:XFD4 A67:XFD1048576 P6:XFD8 A54:C57 E5:XFD5 S9:XFD59 A5:A53 A58:B66 I60:XFD66">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C66">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add row between end of given and start of when
When generating the c# code from the excel tests, "When" can
start immediately after the "Given" section

However when generating the excel from C#, a blank row is
inserted.

So in order to make the test round trippable I have added a
blank row to the spreadsheet.

It would be better if there was an error / warning about this,
probably when creating the C# tests, but possibly in both
directions.
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/Anova.xlsx
+++ b/SampleTests/ExcelTests/Anova.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\SampleTests\ExcelTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7617A041-6382-434B-99C4-F1D987956B0C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F8AF54-76CD-4A5E-BBB1-B42C37CC39EC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -646,10 +646,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC1021"/>
+  <dimension ref="A1:AC1022"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="M54" sqref="M54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2912,18 +2912,12 @@
       <c r="AC53" s="4"/>
     </row>
     <row r="54" spans="1:29" ht="18" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C54" s="11"/>
-      <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
       <c r="G54" s="10"/>
       <c r="H54" s="10"/>
       <c r="I54" s="10"/>
+      <c r="J54" s="10"/>
       <c r="K54" s="10">
         <f>SUM(K12:K53)</f>
         <v>1956.1999999999998</v>
@@ -2933,14 +2927,8 @@
         <f>SUM(M12:M53)</f>
         <v>4294.1000000000004</v>
       </c>
-      <c r="N54" s="10">
-        <f ca="1">AVERAGE(N12:N53)</f>
-        <v>3</v>
-      </c>
-      <c r="O54" s="10">
-        <f>AVERAGE(O12:O53)</f>
-        <v>30</v>
-      </c>
+      <c r="N54" s="10"/>
+      <c r="O54" s="10"/>
       <c r="P54" s="10"/>
       <c r="Q54" s="10"/>
       <c r="R54" s="10"/>
@@ -2957,21 +2945,27 @@
       <c r="AC54" s="4"/>
     </row>
     <row r="55" spans="1:29" ht="18" x14ac:dyDescent="0.25">
-      <c r="A55" s="11"/>
-      <c r="B55" s="11"/>
+      <c r="A55" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
       <c r="E55" s="11"/>
-      <c r="F55" s="10"/>
+      <c r="F55" s="11"/>
       <c r="G55" s="10"/>
       <c r="H55" s="10"/>
       <c r="I55" s="10"/>
-      <c r="J55" s="10"/>
-      <c r="K55" s="10"/>
       <c r="L55" s="10"/>
-      <c r="M55" s="10"/>
-      <c r="N55" s="10"/>
-      <c r="O55" s="10"/>
+      <c r="N55" s="10">
+        <f ca="1">AVERAGE(N12:N53)</f>
+        <v>3</v>
+      </c>
+      <c r="O55" s="10">
+        <f>AVERAGE(O12:O53)</f>
+        <v>30</v>
+      </c>
       <c r="P55" s="10"/>
       <c r="Q55" s="10"/>
       <c r="R55" s="10"/>
@@ -2988,9 +2982,7 @@
       <c r="AC55" s="4"/>
     </row>
     <row r="56" spans="1:29" ht="18" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="A56" s="11"/>
       <c r="B56" s="11"/>
       <c r="C56" s="11"/>
       <c r="D56" s="11"/>
@@ -3021,19 +3013,17 @@
       <c r="AC56" s="4"/>
     </row>
     <row r="57" spans="1:29" ht="18" x14ac:dyDescent="0.25">
-      <c r="A57" s="11"/>
-      <c r="B57" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C57" s="14" t="s">
-        <v>42</v>
-      </c>
+      <c r="A57" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
       <c r="D57" s="11"/>
       <c r="E57" s="11"/>
       <c r="F57" s="10"/>
-      <c r="I57" s="10" t="s">
-        <v>11</v>
-      </c>
+      <c r="G57" s="10"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
       <c r="J57" s="10"/>
       <c r="K57" s="10"/>
       <c r="L57" s="10"/>
@@ -3057,30 +3047,19 @@
     </row>
     <row r="58" spans="1:29" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" s="11"/>
-      <c r="B58" s="11"/>
-      <c r="C58" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D58" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="E58" s="13">
-        <f>J58</f>
-        <v>1956.1999999999998</v>
-      </c>
-      <c r="F58" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G58">
-        <v>1E-3</v>
-      </c>
+      <c r="B58" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="10"/>
       <c r="I58" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J58" s="10">
-        <f>K54</f>
-        <v>1956.1999999999998</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="J58" s="10"/>
       <c r="K58" s="10"/>
       <c r="L58" s="10"/>
       <c r="M58" s="10"/>
@@ -3105,14 +3084,14 @@
       <c r="A59" s="11"/>
       <c r="B59" s="11"/>
       <c r="C59" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D59" s="13" t="s">
         <v>40</v>
       </c>
       <c r="E59" s="13">
-        <f ca="1">J59</f>
-        <v>2</v>
+        <f t="shared" ref="E59:E67" si="21">J59</f>
+        <v>1956.1999999999998</v>
       </c>
       <c r="F59" s="10" t="s">
         <v>45</v>
@@ -3121,11 +3100,11 @@
         <v>1E-3</v>
       </c>
       <c r="I59" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J59" s="10">
-        <f ca="1">N54-1</f>
-        <v>2</v>
+        <f>K54</f>
+        <v>1956.1999999999998</v>
       </c>
       <c r="K59" s="10"/>
       <c r="L59" s="10"/>
@@ -3148,16 +3127,17 @@
       <c r="AC59" s="4"/>
     </row>
     <row r="60" spans="1:29" ht="18" x14ac:dyDescent="0.25">
-      <c r="B60" s="4"/>
+      <c r="A60" s="11"/>
+      <c r="B60" s="11"/>
       <c r="C60" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D60" s="13" t="s">
         <v>40</v>
       </c>
       <c r="E60" s="13">
-        <f ca="1">J60</f>
-        <v>978.09999999999991</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>2</v>
       </c>
       <c r="F60" s="10" t="s">
         <v>45</v>
@@ -3166,20 +3146,20 @@
         <v>1E-3</v>
       </c>
       <c r="I60" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J60" s="10">
-        <f ca="1">J58/J59</f>
-        <v>978.09999999999991</v>
-      </c>
-      <c r="K60" s="4"/>
-      <c r="L60" s="4"/>
-      <c r="M60" s="4"/>
-      <c r="N60" s="4"/>
-      <c r="O60" s="4"/>
-      <c r="P60" s="4"/>
-      <c r="Q60" s="4"/>
-      <c r="R60" s="4"/>
+        <f ca="1">N55-1</f>
+        <v>2</v>
+      </c>
+      <c r="K60" s="10"/>
+      <c r="L60" s="10"/>
+      <c r="M60" s="10"/>
+      <c r="N60" s="10"/>
+      <c r="O60" s="10"/>
+      <c r="P60" s="10"/>
+      <c r="Q60" s="10"/>
+      <c r="R60" s="10"/>
       <c r="S60" s="4"/>
       <c r="T60" s="4"/>
       <c r="U60" s="4"/>
@@ -3195,14 +3175,14 @@
     <row r="61" spans="1:29" ht="18" x14ac:dyDescent="0.25">
       <c r="B61" s="4"/>
       <c r="C61" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D61" s="13" t="s">
         <v>40</v>
       </c>
       <c r="E61" s="13">
-        <f>J61</f>
-        <v>4294.1000000000004</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>978.09999999999991</v>
       </c>
       <c r="F61" s="10" t="s">
         <v>45</v>
@@ -3211,11 +3191,11 @@
         <v>1E-3</v>
       </c>
       <c r="I61" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J61" s="10">
-        <f>M54</f>
-        <v>4294.1000000000004</v>
+        <f ca="1">J59/J60</f>
+        <v>978.09999999999991</v>
       </c>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
@@ -3240,14 +3220,14 @@
     <row r="62" spans="1:29" ht="18" x14ac:dyDescent="0.25">
       <c r="B62" s="4"/>
       <c r="C62" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D62" s="13" t="s">
         <v>40</v>
       </c>
       <c r="E62" s="13">
-        <f ca="1">J62</f>
-        <v>27</v>
+        <f t="shared" si="21"/>
+        <v>4294.1000000000004</v>
       </c>
       <c r="F62" s="10" t="s">
         <v>45</v>
@@ -3256,11 +3236,11 @@
         <v>1E-3</v>
       </c>
       <c r="I62" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J62" s="10">
-        <f ca="1">O54-N54</f>
-        <v>27</v>
+        <f>M54</f>
+        <v>4294.1000000000004</v>
       </c>
       <c r="K62" s="4"/>
       <c r="L62" s="4"/>
@@ -3285,14 +3265,14 @@
     <row r="63" spans="1:29" ht="18" x14ac:dyDescent="0.25">
       <c r="B63" s="4"/>
       <c r="C63" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D63" s="13" t="s">
         <v>40</v>
       </c>
       <c r="E63" s="13">
-        <f ca="1">J63</f>
-        <v>159.04074074074074</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>27</v>
       </c>
       <c r="F63" s="10" t="s">
         <v>45</v>
@@ -3301,11 +3281,11 @@
         <v>1E-3</v>
       </c>
       <c r="I63" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J63" s="10">
-        <f ca="1">J61/J62</f>
-        <v>159.04074074074074</v>
+        <f ca="1">O55-N55</f>
+        <v>27</v>
       </c>
       <c r="K63" s="4"/>
       <c r="L63" s="4"/>
@@ -3330,14 +3310,14 @@
     <row r="64" spans="1:29" ht="18" x14ac:dyDescent="0.25">
       <c r="B64" s="4"/>
       <c r="C64" s="10" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="D64" s="13" t="s">
         <v>40</v>
       </c>
       <c r="E64" s="13">
-        <f ca="1">J64</f>
-        <v>6.1499965068349587</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>159.04074074074074</v>
       </c>
       <c r="F64" s="10" t="s">
         <v>45</v>
@@ -3346,11 +3326,11 @@
         <v>1E-3</v>
       </c>
       <c r="I64" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J64" s="10">
-        <f ca="1">J60/J63</f>
-        <v>6.1499965068349587</v>
+        <f ca="1">J62/J63</f>
+        <v>159.04074074074074</v>
       </c>
       <c r="K64" s="4"/>
       <c r="L64" s="4"/>
@@ -3375,14 +3355,14 @@
     <row r="65" spans="2:29" ht="18" x14ac:dyDescent="0.25">
       <c r="B65" s="4"/>
       <c r="C65" s="10" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="D65" s="13" t="s">
         <v>40</v>
       </c>
       <c r="E65" s="13">
-        <f ca="1">J65</f>
-        <v>6.2966916787415188E-3</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>6.1499965068349587</v>
       </c>
       <c r="F65" s="10" t="s">
         <v>45</v>
@@ -3391,11 +3371,11 @@
         <v>1E-3</v>
       </c>
       <c r="I65" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J65" s="10">
-        <f ca="1">FDIST(J64,J59,J62)</f>
-        <v>6.2966916787415188E-3</v>
+        <f ca="1">J61/J64</f>
+        <v>6.1499965068349587</v>
       </c>
       <c r="K65" s="4"/>
       <c r="L65" s="4"/>
@@ -3420,14 +3400,14 @@
     <row r="66" spans="2:29" ht="18" x14ac:dyDescent="0.25">
       <c r="B66" s="4"/>
       <c r="C66" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D66" s="13" t="s">
         <v>40</v>
       </c>
       <c r="E66" s="13">
-        <f>J66</f>
-        <v>0.31297697710509892</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>6.2966916787415188E-3</v>
       </c>
       <c r="F66" s="10" t="s">
         <v>45</v>
@@ -3436,11 +3416,11 @@
         <v>1E-3</v>
       </c>
       <c r="I66" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J66" s="10">
-        <f>J58/(J58+J61)</f>
-        <v>0.31297697710509892</v>
+        <f ca="1">FDIST(J65,J60,J63)</f>
+        <v>6.2966916787415188E-3</v>
       </c>
       <c r="K66" s="4"/>
       <c r="L66" s="4"/>
@@ -3464,14 +3444,29 @@
     </row>
     <row r="67" spans="2:29" ht="18" x14ac:dyDescent="0.25">
       <c r="B67" s="4"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="4"/>
-      <c r="G67" s="4"/>
-      <c r="H67" s="4"/>
-      <c r="I67" s="4"/>
-      <c r="J67" s="4"/>
+      <c r="C67" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D67" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E67" s="13">
+        <f t="shared" si="21"/>
+        <v>0.31297697710509892</v>
+      </c>
+      <c r="F67" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G67">
+        <v>1E-3</v>
+      </c>
+      <c r="I67" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J67" s="10">
+        <f>J59/(J59+J62)</f>
+        <v>0.31297697710509892</v>
+      </c>
       <c r="K67" s="4"/>
       <c r="L67" s="4"/>
       <c r="M67" s="4"/>
@@ -32112,13 +32107,43 @@
       <c r="AB1021" s="4"/>
       <c r="AC1021" s="4"/>
     </row>
+    <row r="1022" spans="2:29" ht="18" x14ac:dyDescent="0.25">
+      <c r="B1022" s="4"/>
+      <c r="C1022" s="4"/>
+      <c r="D1022" s="4"/>
+      <c r="E1022" s="4"/>
+      <c r="F1022" s="4"/>
+      <c r="G1022" s="4"/>
+      <c r="H1022" s="4"/>
+      <c r="I1022" s="4"/>
+      <c r="J1022" s="4"/>
+      <c r="K1022" s="4"/>
+      <c r="L1022" s="4"/>
+      <c r="M1022" s="4"/>
+      <c r="N1022" s="4"/>
+      <c r="O1022" s="4"/>
+      <c r="P1022" s="4"/>
+      <c r="Q1022" s="4"/>
+      <c r="R1022" s="4"/>
+      <c r="S1022" s="4"/>
+      <c r="T1022" s="4"/>
+      <c r="U1022" s="4"/>
+      <c r="V1022" s="4"/>
+      <c r="W1022" s="4"/>
+      <c r="X1022" s="4"/>
+      <c r="Y1022" s="4"/>
+      <c r="Z1022" s="4"/>
+      <c r="AA1022" s="4"/>
+      <c r="AB1022" s="4"/>
+      <c r="AC1022" s="4"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD4 A67:XFD1048576 P6:XFD8 A54:C57 E5:XFD5 S9:XFD59 A5:A53 A58:B66 I60:XFD66">
+  <conditionalFormatting sqref="A1:XFD4 A68:XFD1048576 P6:XFD8 A55:C58 E5:XFD5 S9:XFD60 A5:A54 A59:B67 I61:XFD67">
     <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C60:C66">
+  <conditionalFormatting sqref="C61:C67">
     <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>""""""</formula>
     </cfRule>

</xml_diff>

<commit_message>
Add notes / comments to sample excel files
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/Anova.xlsx
+++ b/SampleTests/ExcelTests/Anova.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\SampleTests\ExcelTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC0A5EB-6C2C-40B5-92E0-A6AF2574F93E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{17F64B84-0C97-40FA-AC57-515F7BE35447}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="54">
   <si>
     <t>Example from:</t>
   </si>
@@ -161,6 +161,27 @@
   </si>
   <si>
     <t>"Alderbrook School"</t>
+  </si>
+  <si>
+    <t>As long as there is a gap after the property columns, you can use the rest of the sheet to add notes and do calculations</t>
+  </si>
+  <si>
+    <t>This example / end to end test shows the following</t>
+  </si>
+  <si>
+    <t>Nested Property Setup</t>
+  </si>
+  <si>
+    <t>Table property setup (using "table of"</t>
+  </si>
+  <si>
+    <t>Nested assertions</t>
+  </si>
+  <si>
+    <t>Calculations in the assertions (which do not get overwrttien when round tripping)</t>
+  </si>
+  <si>
+    <t>Tables within tables (the last nested table can use the "table of" syntax, but higher up the hierarchy the "PropertyName(index) of" syntax must be used</t>
   </si>
 </sst>
 </file>
@@ -204,11 +225,46 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="20">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -255,6 +311,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -288,26 +351,44 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
       <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
       <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -624,8 +705,8 @@
   </sheetPr>
   <dimension ref="A1:O1022"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -667,18 +748,27 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="I4" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="5" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
@@ -687,6 +777,9 @@
       <c r="D5" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="I5" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="6" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C6" s="1" t="s">
@@ -695,11 +788,17 @@
       <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="I6" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="7" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D7" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="I7" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="8" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="E8" s="1" t="s">
@@ -715,6 +814,9 @@
       </c>
       <c r="F9" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
@@ -3163,38 +3265,72 @@
     <row r="1021" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="1022" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="A1:XFD2 A3:G5 J3:XFD5 A6:XFD1048576">
+    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
       <formula>"Assert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
       <formula>"Given a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
       <formula>"Specification"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="9" priority="5" operator="beginsWith" text="With Properties">
+    <cfRule type="beginsWith" dxfId="15" priority="15" operator="beginsWith" text="With Properties">
       <formula>LEFT(A1,LEN("With Properties"))="With Properties"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="8" priority="6" operator="endsWith" text=" table of">
+    <cfRule type="endsWith" dxfId="14" priority="16" operator="endsWith" text=" table of">
       <formula>RIGHT(A1,LEN(" table of"))=" table of"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="7" priority="7" operator="endsWith" text=" of">
+    <cfRule type="endsWith" dxfId="13" priority="17" operator="endsWith" text=" of">
       <formula>RIGHT(A1,LEN(" of"))=" of"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="12" priority="18">
       <formula>AND((RIGHT(A1048576, 3) = " of"), A2 = "With Properties")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="9">
+    <cfRule type="expression" dxfId="11" priority="19">
       <formula>AND(RIGHT(XFD1, 3) = " of", A2 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1048576">
+  <conditionalFormatting sqref="A1:XFD2 A3:G5 J3:XFD5 A6:XFD1048576">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="20">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:I5">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+      <formula>"Assert"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>"Given a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>"Specification"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="5" priority="5" operator="beginsWith" text="With Properties">
+      <formula>LEFT(H3,LEN("With Properties"))="With Properties"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="4" priority="6" operator="endsWith" text=" table of">
+      <formula>RIGHT(H3,LEN(" table of"))=" table of"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="3" priority="7" operator="endsWith" text=" of">
+      <formula>RIGHT(H3,LEN(" of"))=" of"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="8">
+      <formula>AND((RIGHT(H2, 3) = " of"), H4 = "With Properties")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="9">
+      <formula>AND(RIGHT(G3, 3) = " of", H4 = "With Properties")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:I5">
     <cfRule type="notContainsBlanks" dxfId="0" priority="10">
-      <formula>LEN(TRIM(A1))&gt;0</formula>
+      <formula>LEN(TRIM(H3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>

<commit_message>
Convert Anova end to end test to use new list of syntax
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/Anova.xlsx
+++ b/SampleTests/ExcelTests/Anova.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\SampleTests\ExcelTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{17F64B84-0C97-40FA-AC57-515F7BE35447}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CFA5DECF-1ADD-48DC-BC3D-38EC57127370}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="55">
   <si>
     <t>Example from:</t>
   </si>
@@ -100,9 +100,6 @@
     <t>With Properties</t>
   </si>
   <si>
-    <t>Groups(0) of</t>
-  </si>
-  <si>
     <t>Name of</t>
   </si>
   <si>
@@ -118,12 +115,6 @@
     <t>Value of</t>
   </si>
   <si>
-    <t>Groups(1) of</t>
-  </si>
-  <si>
-    <t>Groups(2) of</t>
-  </si>
-  <si>
     <t>When</t>
   </si>
   <si>
@@ -182,17 +173,36 @@
   </si>
   <si>
     <t>Tables within tables (the last nested table can use the "table of" syntax, but higher up the hierarchy the "PropertyName(index) of" syntax must be used</t>
+  </si>
+  <si>
+    <t>Groups list of</t>
+  </si>
+  <si>
+    <t>With Item</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>Average</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -215,17 +225,554 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="86">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -703,10 +1250,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O1022"/>
+  <dimension ref="A1:O1020"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:I7"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -738,7 +1285,7 @@
         <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
@@ -747,7 +1294,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I2" s="2"/>
+    </row>
     <row r="3" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>23</v>
@@ -756,10 +1305,10 @@
         <v>24</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
@@ -767,56 +1316,56 @@
         <v>25</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D7" s="1" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="E8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="H9" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
@@ -826,7 +1375,7 @@
     </row>
     <row r="11" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="F11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>3</v>
@@ -862,23 +1411,23 @@
         <v>99.2</v>
       </c>
       <c r="I12" s="1">
-        <f>AVERAGE(F$12:F$53)</f>
+        <f t="shared" ref="I12:I21" si="1">AVERAGE(F$12:F$51)</f>
         <v>101.7</v>
       </c>
       <c r="J12" s="1">
-        <f t="shared" ref="J12:J21" si="1">H12-I12</f>
+        <f t="shared" ref="J12:J21" si="2">H12-I12</f>
         <v>-2.5</v>
       </c>
       <c r="K12" s="1">
-        <f t="shared" ref="K12:K21" si="2">J12^2</f>
+        <f t="shared" ref="K12:K21" si="3">J12^2</f>
         <v>6.25</v>
       </c>
       <c r="L12" s="1">
-        <f t="shared" ref="L12:L21" si="3">F12-H12</f>
+        <f t="shared" ref="L12:L21" si="4">F12-H12</f>
         <v>-9.2000000000000028</v>
       </c>
       <c r="M12" s="1">
-        <f t="shared" ref="M12:M21" si="4">L12^2</f>
+        <f t="shared" ref="M12:M21" si="5">L12^2</f>
         <v>84.640000000000057</v>
       </c>
       <c r="N12" s="1">
@@ -886,7 +1435,7 @@
         <v>3</v>
       </c>
       <c r="O12" s="1">
-        <f>COUNT(F$12:F$53)</f>
+        <f t="shared" ref="O12:O21" si="6">COUNT(F$12:F$51)</f>
         <v>30</v>
       </c>
     </row>
@@ -899,23 +1448,23 @@
         <v>99.2</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" ref="I13:I21" si="5">AVERAGE(F$12:F$53)</f>
+        <f t="shared" si="1"/>
         <v>101.7</v>
       </c>
       <c r="J13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.5</v>
       </c>
       <c r="K13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.25</v>
       </c>
       <c r="L13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-12.200000000000003</v>
       </c>
       <c r="M13" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>148.84000000000006</v>
       </c>
       <c r="N13" s="1">
@@ -923,7 +1472,7 @@
         <v>3</v>
       </c>
       <c r="O13" s="1">
-        <f t="shared" ref="O13:O21" si="6">COUNT(F$12:F$53)</f>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
     </row>
@@ -936,23 +1485,23 @@
         <v>99.2</v>
       </c>
       <c r="I14" s="1">
+        <f t="shared" si="1"/>
+        <v>101.7</v>
+      </c>
+      <c r="J14" s="1">
+        <f t="shared" si="2"/>
+        <v>-2.5</v>
+      </c>
+      <c r="K14" s="1">
+        <f t="shared" si="3"/>
+        <v>6.25</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="4"/>
+        <v>-6.2000000000000028</v>
+      </c>
+      <c r="M14" s="1">
         <f t="shared" si="5"/>
-        <v>101.7</v>
-      </c>
-      <c r="J14" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.5</v>
-      </c>
-      <c r="K14" s="1">
-        <f t="shared" si="2"/>
-        <v>6.25</v>
-      </c>
-      <c r="L14" s="1">
-        <f t="shared" si="3"/>
-        <v>-6.2000000000000028</v>
-      </c>
-      <c r="M14" s="1">
-        <f t="shared" si="4"/>
         <v>38.440000000000033</v>
       </c>
       <c r="N14" s="1">
@@ -973,23 +1522,23 @@
         <v>99.2</v>
       </c>
       <c r="I15" s="1">
+        <f t="shared" si="1"/>
+        <v>101.7</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" si="2"/>
+        <v>-2.5</v>
+      </c>
+      <c r="K15" s="1">
+        <f t="shared" si="3"/>
+        <v>6.25</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="4"/>
+        <v>15.799999999999997</v>
+      </c>
+      <c r="M15" s="1">
         <f t="shared" si="5"/>
-        <v>101.7</v>
-      </c>
-      <c r="J15" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.5</v>
-      </c>
-      <c r="K15" s="1">
-        <f t="shared" si="2"/>
-        <v>6.25</v>
-      </c>
-      <c r="L15" s="1">
-        <f t="shared" si="3"/>
-        <v>15.799999999999997</v>
-      </c>
-      <c r="M15" s="1">
-        <f t="shared" si="4"/>
         <v>249.6399999999999</v>
       </c>
       <c r="N15" s="1">
@@ -1010,23 +1559,23 @@
         <v>99.2</v>
       </c>
       <c r="I16" s="1">
+        <f t="shared" si="1"/>
+        <v>101.7</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="2"/>
+        <v>-2.5</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="3"/>
+        <v>6.25</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" si="4"/>
+        <v>-2.2000000000000028</v>
+      </c>
+      <c r="M16" s="1">
         <f t="shared" si="5"/>
-        <v>101.7</v>
-      </c>
-      <c r="J16" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.5</v>
-      </c>
-      <c r="K16" s="1">
-        <f t="shared" si="2"/>
-        <v>6.25</v>
-      </c>
-      <c r="L16" s="1">
-        <f t="shared" si="3"/>
-        <v>-2.2000000000000028</v>
-      </c>
-      <c r="M16" s="1">
-        <f t="shared" si="4"/>
         <v>4.8400000000000123</v>
       </c>
       <c r="N16" s="1">
@@ -1038,7 +1587,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F17" s="1">
         <v>85</v>
       </c>
@@ -1047,23 +1596,23 @@
         <v>99.2</v>
       </c>
       <c r="I17" s="1">
+        <f t="shared" si="1"/>
+        <v>101.7</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="2"/>
+        <v>-2.5</v>
+      </c>
+      <c r="K17" s="1">
+        <f t="shared" si="3"/>
+        <v>6.25</v>
+      </c>
+      <c r="L17" s="1">
+        <f t="shared" si="4"/>
+        <v>-14.200000000000003</v>
+      </c>
+      <c r="M17" s="1">
         <f t="shared" si="5"/>
-        <v>101.7</v>
-      </c>
-      <c r="J17" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.5</v>
-      </c>
-      <c r="K17" s="1">
-        <f t="shared" si="2"/>
-        <v>6.25</v>
-      </c>
-      <c r="L17" s="1">
-        <f t="shared" si="3"/>
-        <v>-14.200000000000003</v>
-      </c>
-      <c r="M17" s="1">
-        <f t="shared" si="4"/>
         <v>201.64000000000007</v>
       </c>
       <c r="N17" s="1">
@@ -1075,7 +1624,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F18" s="1">
         <v>102</v>
       </c>
@@ -1084,23 +1633,23 @@
         <v>99.2</v>
       </c>
       <c r="I18" s="1">
+        <f t="shared" si="1"/>
+        <v>101.7</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="2"/>
+        <v>-2.5</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" si="3"/>
+        <v>6.25</v>
+      </c>
+      <c r="L18" s="1">
+        <f t="shared" si="4"/>
+        <v>2.7999999999999972</v>
+      </c>
+      <c r="M18" s="1">
         <f t="shared" si="5"/>
-        <v>101.7</v>
-      </c>
-      <c r="J18" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.5</v>
-      </c>
-      <c r="K18" s="1">
-        <f t="shared" si="2"/>
-        <v>6.25</v>
-      </c>
-      <c r="L18" s="1">
-        <f t="shared" si="3"/>
-        <v>2.7999999999999972</v>
-      </c>
-      <c r="M18" s="1">
-        <f t="shared" si="4"/>
         <v>7.8399999999999839</v>
       </c>
       <c r="N18" s="1">
@@ -1112,7 +1661,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F19" s="1">
         <v>110</v>
       </c>
@@ -1121,23 +1670,23 @@
         <v>99.2</v>
       </c>
       <c r="I19" s="1">
+        <f t="shared" si="1"/>
+        <v>101.7</v>
+      </c>
+      <c r="J19" s="1">
+        <f t="shared" si="2"/>
+        <v>-2.5</v>
+      </c>
+      <c r="K19" s="1">
+        <f t="shared" si="3"/>
+        <v>6.25</v>
+      </c>
+      <c r="L19" s="1">
+        <f t="shared" si="4"/>
+        <v>10.799999999999997</v>
+      </c>
+      <c r="M19" s="1">
         <f t="shared" si="5"/>
-        <v>101.7</v>
-      </c>
-      <c r="J19" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.5</v>
-      </c>
-      <c r="K19" s="1">
-        <f t="shared" si="2"/>
-        <v>6.25</v>
-      </c>
-      <c r="L19" s="1">
-        <f t="shared" si="3"/>
-        <v>10.799999999999997</v>
-      </c>
-      <c r="M19" s="1">
-        <f t="shared" si="4"/>
         <v>116.63999999999994</v>
       </c>
       <c r="N19" s="1">
@@ -1149,7 +1698,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F20" s="1">
         <v>111</v>
       </c>
@@ -1158,23 +1707,23 @@
         <v>99.2</v>
       </c>
       <c r="I20" s="1">
+        <f t="shared" si="1"/>
+        <v>101.7</v>
+      </c>
+      <c r="J20" s="1">
+        <f t="shared" si="2"/>
+        <v>-2.5</v>
+      </c>
+      <c r="K20" s="1">
+        <f t="shared" si="3"/>
+        <v>6.25</v>
+      </c>
+      <c r="L20" s="1">
+        <f t="shared" si="4"/>
+        <v>11.799999999999997</v>
+      </c>
+      <c r="M20" s="1">
         <f t="shared" si="5"/>
-        <v>101.7</v>
-      </c>
-      <c r="J20" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.5</v>
-      </c>
-      <c r="K20" s="1">
-        <f t="shared" si="2"/>
-        <v>6.25</v>
-      </c>
-      <c r="L20" s="1">
-        <f t="shared" si="3"/>
-        <v>11.799999999999997</v>
-      </c>
-      <c r="M20" s="1">
-        <f t="shared" si="4"/>
         <v>139.23999999999992</v>
       </c>
       <c r="N20" s="1">
@@ -1186,7 +1735,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F21" s="1">
         <v>102</v>
       </c>
@@ -1195,23 +1744,23 @@
         <v>99.2</v>
       </c>
       <c r="I21" s="1">
+        <f t="shared" si="1"/>
+        <v>101.7</v>
+      </c>
+      <c r="J21" s="1">
+        <f t="shared" si="2"/>
+        <v>-2.5</v>
+      </c>
+      <c r="K21" s="1">
+        <f t="shared" si="3"/>
+        <v>6.25</v>
+      </c>
+      <c r="L21" s="1">
+        <f t="shared" si="4"/>
+        <v>2.7999999999999972</v>
+      </c>
+      <c r="M21" s="1">
         <f t="shared" si="5"/>
-        <v>101.7</v>
-      </c>
-      <c r="J21" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.5</v>
-      </c>
-      <c r="K21" s="1">
-        <f t="shared" si="2"/>
-        <v>6.25</v>
-      </c>
-      <c r="L21" s="1">
-        <f t="shared" si="3"/>
-        <v>2.7999999999999972</v>
-      </c>
-      <c r="M21" s="1">
-        <f t="shared" si="4"/>
         <v>7.8399999999999839</v>
       </c>
       <c r="N21" s="1">
@@ -1223,566 +1772,624 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C22" s="1" t="s">
-        <v>32</v>
-      </c>
+    <row r="22" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D22" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D23" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F25" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E24" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E25" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F25" s="1" t="s">
+    <row r="26" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F26" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F26" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F27" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F27" s="1">
+        <v>135</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" ref="H27:H36" si="7">AVERAGE(F$27:F$36)</f>
+        <v>112.6</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" ref="I27:I36" si="8">AVERAGE(F$12:F$51)</f>
+        <v>101.7</v>
+      </c>
+      <c r="J27" s="1">
+        <f t="shared" ref="J27:J36" si="9">H27-I27</f>
+        <v>10.899999999999991</v>
+      </c>
+      <c r="K27" s="1">
+        <f t="shared" ref="K27:K36" si="10">J27^2</f>
+        <v>118.80999999999982</v>
+      </c>
+      <c r="L27" s="1">
+        <f t="shared" ref="L27:L36" si="11">F27-H27</f>
+        <v>22.400000000000006</v>
+      </c>
+      <c r="M27" s="1">
+        <f t="shared" ref="M27:M36" si="12">L27^2</f>
+        <v>501.76000000000028</v>
+      </c>
+      <c r="N27" s="1">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("countunique(A$4:A$33)"),3)</f>
+        <v>3</v>
+      </c>
+      <c r="O27" s="1">
+        <f t="shared" ref="O27:O36" si="13">COUNT(F$12:F$51)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F28" s="1">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="H28" s="1">
-        <f t="shared" ref="H28:H37" si="7">AVERAGE(F$28:F$37)</f>
+        <f t="shared" si="7"/>
         <v>112.6</v>
       </c>
       <c r="I28" s="1">
-        <f>AVERAGE(F$12:F$53)</f>
+        <f t="shared" si="8"/>
         <v>101.7</v>
       </c>
       <c r="J28" s="1">
-        <f t="shared" ref="J28:J37" si="8">H28-I28</f>
+        <f t="shared" si="9"/>
         <v>10.899999999999991</v>
       </c>
       <c r="K28" s="1">
-        <f t="shared" ref="K28:K37" si="9">J28^2</f>
+        <f t="shared" si="10"/>
         <v>118.80999999999982</v>
       </c>
       <c r="L28" s="1">
-        <f t="shared" ref="L28:L37" si="10">F28-H28</f>
-        <v>22.400000000000006</v>
+        <f t="shared" si="11"/>
+        <v>12.400000000000006</v>
       </c>
       <c r="M28" s="1">
-        <f t="shared" ref="M28:M37" si="11">L28^2</f>
-        <v>501.76000000000028</v>
+        <f t="shared" si="12"/>
+        <v>153.76000000000013</v>
       </c>
       <c r="N28" s="1">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("countunique(A$4:A$33)"),3)</f>
         <v>3</v>
       </c>
       <c r="O28" s="1">
-        <f t="shared" ref="O28:O37" si="12">COUNT(F$12:F$53)</f>
+        <f t="shared" si="13"/>
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F29" s="1">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="H29" s="1">
         <f t="shared" si="7"/>
         <v>112.6</v>
       </c>
       <c r="I29" s="1">
-        <f t="shared" ref="I29:I37" si="13">AVERAGE(F$12:F$53)</f>
+        <f t="shared" si="8"/>
         <v>101.7</v>
       </c>
       <c r="J29" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10.899999999999991</v>
       </c>
       <c r="K29" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>118.80999999999982</v>
       </c>
       <c r="L29" s="1">
-        <f t="shared" si="10"/>
-        <v>12.400000000000006</v>
+        <f t="shared" si="11"/>
+        <v>-5.5999999999999943</v>
       </c>
       <c r="M29" s="1">
-        <f t="shared" si="11"/>
-        <v>153.76000000000013</v>
+        <f t="shared" si="12"/>
+        <v>31.359999999999935</v>
       </c>
       <c r="N29" s="1">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("countunique(A$4:A$33)"),3)</f>
         <v>3</v>
       </c>
       <c r="O29" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F30" s="1">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="H30" s="1">
         <f t="shared" si="7"/>
         <v>112.6</v>
       </c>
       <c r="I30" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>101.7</v>
       </c>
       <c r="J30" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10.899999999999991</v>
       </c>
       <c r="K30" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>118.80999999999982</v>
       </c>
       <c r="L30" s="1">
-        <f t="shared" si="10"/>
-        <v>-5.5999999999999943</v>
+        <f t="shared" si="11"/>
+        <v>-16.599999999999994</v>
       </c>
       <c r="M30" s="1">
-        <f t="shared" si="11"/>
-        <v>31.359999999999935</v>
+        <f t="shared" si="12"/>
+        <v>275.55999999999983</v>
       </c>
       <c r="N30" s="1">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("countunique(A$4:A$33)"),3)</f>
         <v>3</v>
       </c>
       <c r="O30" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F31" s="1">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="H31" s="1">
         <f t="shared" si="7"/>
         <v>112.6</v>
       </c>
       <c r="I31" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>101.7</v>
       </c>
       <c r="J31" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10.899999999999991</v>
       </c>
       <c r="K31" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>118.80999999999982</v>
       </c>
       <c r="L31" s="1">
-        <f t="shared" si="10"/>
-        <v>-16.599999999999994</v>
+        <f t="shared" si="11"/>
+        <v>1.4000000000000057</v>
       </c>
       <c r="M31" s="1">
-        <f t="shared" si="11"/>
-        <v>275.55999999999983</v>
+        <f t="shared" si="12"/>
+        <v>1.960000000000016</v>
       </c>
       <c r="N31" s="1">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("countunique(A$4:A$33)"),3)</f>
         <v>3</v>
       </c>
       <c r="O31" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F32" s="1">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="H32" s="1">
         <f t="shared" si="7"/>
         <v>112.6</v>
       </c>
       <c r="I32" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>101.7</v>
       </c>
       <c r="J32" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10.899999999999991</v>
       </c>
       <c r="K32" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>118.80999999999982</v>
       </c>
       <c r="L32" s="1">
-        <f t="shared" si="10"/>
-        <v>1.4000000000000057</v>
+        <f t="shared" si="11"/>
+        <v>12.400000000000006</v>
       </c>
       <c r="M32" s="1">
-        <f t="shared" si="11"/>
-        <v>1.960000000000016</v>
+        <f t="shared" si="12"/>
+        <v>153.76000000000013</v>
       </c>
       <c r="N32" s="1">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("countunique(A$4:A$33)"),3)</f>
         <v>3</v>
       </c>
       <c r="O32" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F33" s="1">
-        <v>125</v>
+        <v>94</v>
       </c>
       <c r="H33" s="1">
         <f t="shared" si="7"/>
         <v>112.6</v>
       </c>
       <c r="I33" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>101.7</v>
       </c>
       <c r="J33" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10.899999999999991</v>
       </c>
       <c r="K33" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>118.80999999999982</v>
       </c>
       <c r="L33" s="1">
-        <f t="shared" si="10"/>
-        <v>12.400000000000006</v>
+        <f t="shared" si="11"/>
+        <v>-18.599999999999994</v>
       </c>
       <c r="M33" s="1">
-        <f t="shared" si="11"/>
-        <v>153.76000000000013</v>
+        <f t="shared" si="12"/>
+        <v>345.95999999999981</v>
       </c>
       <c r="N33" s="1">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("countunique(A$4:A$33)"),3)</f>
         <v>3</v>
       </c>
       <c r="O33" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F34" s="1">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="H34" s="1">
         <f t="shared" si="7"/>
         <v>112.6</v>
       </c>
       <c r="I34" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>101.7</v>
       </c>
       <c r="J34" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10.899999999999991</v>
       </c>
       <c r="K34" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>118.80999999999982</v>
       </c>
       <c r="L34" s="1">
-        <f t="shared" si="10"/>
-        <v>-18.599999999999994</v>
+        <f t="shared" si="11"/>
+        <v>10.400000000000006</v>
       </c>
       <c r="M34" s="1">
-        <f t="shared" si="11"/>
-        <v>345.95999999999981</v>
+        <f t="shared" si="12"/>
+        <v>108.16000000000012</v>
       </c>
       <c r="N34" s="1">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("countunique(A$4:A$33)"),3)</f>
         <v>3</v>
       </c>
       <c r="O34" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F35" s="1">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="H35" s="1">
         <f t="shared" si="7"/>
         <v>112.6</v>
       </c>
       <c r="I35" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>101.7</v>
       </c>
       <c r="J35" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10.899999999999991</v>
       </c>
       <c r="K35" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>118.80999999999982</v>
       </c>
       <c r="L35" s="1">
-        <f t="shared" si="10"/>
-        <v>10.400000000000006</v>
+        <f t="shared" si="11"/>
+        <v>-1.5999999999999943</v>
       </c>
       <c r="M35" s="1">
-        <f t="shared" si="11"/>
-        <v>108.16000000000012</v>
+        <f t="shared" si="12"/>
+        <v>2.5599999999999818</v>
       </c>
       <c r="N35" s="1">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("countunique(A$4:A$33)"),3)</f>
         <v>3</v>
       </c>
       <c r="O35" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F36" s="1">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="H36" s="1">
         <f t="shared" si="7"/>
         <v>112.6</v>
       </c>
       <c r="I36" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>101.7</v>
       </c>
       <c r="J36" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10.899999999999991</v>
       </c>
       <c r="K36" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>118.80999999999982</v>
       </c>
       <c r="L36" s="1">
-        <f t="shared" si="10"/>
-        <v>-1.5999999999999943</v>
+        <f t="shared" si="11"/>
+        <v>-16.599999999999994</v>
       </c>
       <c r="M36" s="1">
-        <f t="shared" si="11"/>
-        <v>2.5599999999999818</v>
+        <f t="shared" si="12"/>
+        <v>275.55999999999983</v>
       </c>
       <c r="N36" s="1">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("countunique(A$4:A$33)"),3)</f>
         <v>3</v>
       </c>
       <c r="O36" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F37" s="1">
-        <v>96</v>
-      </c>
-      <c r="H37" s="1">
-        <f t="shared" si="7"/>
-        <v>112.6</v>
-      </c>
-      <c r="I37" s="1">
-        <f t="shared" si="13"/>
+    <row r="37" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D37" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E39" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F40" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F41" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F42" s="1">
+        <v>93</v>
+      </c>
+      <c r="H42" s="1">
+        <f t="shared" ref="H42:H51" si="14">AVERAGE(F$42:F$51)</f>
+        <v>93.3</v>
+      </c>
+      <c r="I42" s="1">
+        <f t="shared" ref="I42:I51" si="15">AVERAGE(F$12:F$51)</f>
         <v>101.7</v>
       </c>
-      <c r="J37" s="1">
-        <f t="shared" si="8"/>
-        <v>10.899999999999991</v>
-      </c>
-      <c r="K37" s="1">
-        <f t="shared" si="9"/>
-        <v>118.80999999999982</v>
-      </c>
-      <c r="L37" s="1">
-        <f t="shared" si="10"/>
-        <v>-16.599999999999994</v>
-      </c>
-      <c r="M37" s="1">
-        <f t="shared" si="11"/>
-        <v>275.55999999999983</v>
-      </c>
-      <c r="N37" s="1">
+      <c r="J42" s="1">
+        <f t="shared" ref="J42:J51" si="16">H42-I42</f>
+        <v>-8.4000000000000057</v>
+      </c>
+      <c r="K42" s="1">
+        <f t="shared" ref="K42:K51" si="17">J42^2</f>
+        <v>70.560000000000102</v>
+      </c>
+      <c r="L42" s="1">
+        <f t="shared" ref="L42:L51" si="18">F42-H42</f>
+        <v>-0.29999999999999716</v>
+      </c>
+      <c r="M42" s="1">
+        <f t="shared" ref="M42:M51" si="19">L42^2</f>
+        <v>8.999999999999829E-2</v>
+      </c>
+      <c r="N42" s="1">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("countunique(A$4:A$33)"),3)</f>
         <v>3</v>
       </c>
-      <c r="O37" s="1">
-        <f t="shared" si="12"/>
+      <c r="O42" s="1">
+        <f t="shared" ref="O42:O51" si="20">COUNT(F$12:F$51)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C38" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D39" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E40" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="41" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E41" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F41" s="1" t="s">
+    <row r="43" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F43" s="1">
+        <v>101</v>
+      </c>
+      <c r="H43" s="1">
+        <f t="shared" si="14"/>
+        <v>93.3</v>
+      </c>
+      <c r="I43" s="1">
+        <f t="shared" si="15"/>
+        <v>101.7</v>
+      </c>
+      <c r="J43" s="1">
+        <f t="shared" si="16"/>
+        <v>-8.4000000000000057</v>
+      </c>
+      <c r="K43" s="1">
+        <f t="shared" si="17"/>
+        <v>70.560000000000102</v>
+      </c>
+      <c r="L43" s="1">
+        <f t="shared" si="18"/>
+        <v>7.7000000000000028</v>
+      </c>
+      <c r="M43" s="1">
+        <f t="shared" si="19"/>
+        <v>59.290000000000042</v>
+      </c>
+      <c r="N43" s="1">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("countunique(A$4:A$33)"),3)</f>
+        <v>3</v>
+      </c>
+      <c r="O43" s="1">
+        <f t="shared" si="20"/>
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F42" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="43" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F43" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="44" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F44" s="1">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="H44" s="1">
-        <f t="shared" ref="H44:H53" si="14">AVERAGE(F$44:F$53)</f>
+        <f t="shared" si="14"/>
         <v>93.3</v>
       </c>
       <c r="I44" s="1">
-        <f>AVERAGE(F$12:F$53)</f>
+        <f t="shared" si="15"/>
         <v>101.7</v>
       </c>
       <c r="J44" s="1">
-        <f t="shared" ref="J44:J53" si="15">H44-I44</f>
+        <f t="shared" si="16"/>
         <v>-8.4000000000000057</v>
       </c>
       <c r="K44" s="1">
-        <f t="shared" ref="K44:K53" si="16">J44^2</f>
+        <f t="shared" si="17"/>
         <v>70.560000000000102</v>
       </c>
       <c r="L44" s="1">
-        <f t="shared" ref="L44:L53" si="17">F44-H44</f>
-        <v>-0.29999999999999716</v>
+        <f t="shared" si="18"/>
+        <v>-19.299999999999997</v>
       </c>
       <c r="M44" s="1">
-        <f t="shared" ref="M44:M53" si="18">L44^2</f>
-        <v>8.999999999999829E-2</v>
+        <f t="shared" si="19"/>
+        <v>372.4899999999999</v>
       </c>
       <c r="N44" s="1">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("countunique(A$4:A$33)"),3)</f>
         <v>3</v>
       </c>
       <c r="O44" s="1">
-        <f t="shared" ref="O44:O53" si="19">COUNT(F$12:F$53)</f>
+        <f t="shared" si="20"/>
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F45" s="1">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="H45" s="1">
         <f t="shared" si="14"/>
         <v>93.3</v>
       </c>
       <c r="I45" s="1">
-        <f t="shared" ref="I45:I53" si="20">AVERAGE(F$12:F$53)</f>
+        <f t="shared" si="15"/>
         <v>101.7</v>
       </c>
       <c r="J45" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-8.4000000000000057</v>
       </c>
       <c r="K45" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>70.560000000000102</v>
       </c>
       <c r="L45" s="1">
-        <f t="shared" si="17"/>
-        <v>7.7000000000000028</v>
+        <f t="shared" si="18"/>
+        <v>-6.2999999999999972</v>
       </c>
       <c r="M45" s="1">
-        <f t="shared" si="18"/>
-        <v>59.290000000000042</v>
+        <f t="shared" si="19"/>
+        <v>39.689999999999962</v>
       </c>
       <c r="N45" s="1">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("countunique(A$4:A$33)"),3)</f>
         <v>3</v>
       </c>
       <c r="O45" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F46" s="1">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H46" s="1">
         <f t="shared" si="14"/>
         <v>93.3</v>
       </c>
       <c r="I46" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>101.7</v>
       </c>
       <c r="J46" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-8.4000000000000057</v>
       </c>
       <c r="K46" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>70.560000000000102</v>
       </c>
       <c r="L46" s="1">
-        <f t="shared" si="17"/>
-        <v>-19.299999999999997</v>
+        <f t="shared" si="18"/>
+        <v>-17.299999999999997</v>
       </c>
       <c r="M46" s="1">
-        <f t="shared" si="18"/>
-        <v>372.4899999999999</v>
+        <f t="shared" si="19"/>
+        <v>299.28999999999991</v>
       </c>
       <c r="N46" s="1">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("countunique(A$4:A$33)"),3)</f>
         <v>3</v>
       </c>
       <c r="O46" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F47" s="1">
         <v>87</v>
       </c>
@@ -1791,23 +2398,23 @@
         <v>93.3</v>
       </c>
       <c r="I47" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>101.7</v>
       </c>
       <c r="J47" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-8.4000000000000057</v>
       </c>
       <c r="K47" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>70.560000000000102</v>
       </c>
       <c r="L47" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-6.2999999999999972</v>
       </c>
       <c r="M47" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>39.689999999999962</v>
       </c>
       <c r="N47" s="1">
@@ -1815,500 +2422,437 @@
         <v>3</v>
       </c>
       <c r="O47" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="3:15" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F48" s="1">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="H48" s="1">
         <f t="shared" si="14"/>
         <v>93.3</v>
       </c>
       <c r="I48" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>101.7</v>
       </c>
       <c r="J48" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-8.4000000000000057</v>
       </c>
       <c r="K48" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>70.560000000000102</v>
       </c>
       <c r="L48" s="1">
-        <f t="shared" si="17"/>
-        <v>-17.299999999999997</v>
+        <f t="shared" si="18"/>
+        <v>4.7000000000000028</v>
       </c>
       <c r="M48" s="1">
-        <f t="shared" si="18"/>
-        <v>299.28999999999991</v>
+        <f t="shared" si="19"/>
+        <v>22.090000000000028</v>
       </c>
       <c r="N48" s="1">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("countunique(A$4:A$33)"),3)</f>
         <v>3</v>
       </c>
       <c r="O48" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F49" s="1">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="H49" s="1">
         <f t="shared" si="14"/>
         <v>93.3</v>
       </c>
       <c r="I49" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>101.7</v>
       </c>
       <c r="J49" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-8.4000000000000057</v>
       </c>
       <c r="K49" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>70.560000000000102</v>
       </c>
       <c r="L49" s="1">
-        <f t="shared" si="17"/>
-        <v>-6.2999999999999972</v>
+        <f t="shared" si="18"/>
+        <v>14.700000000000003</v>
       </c>
       <c r="M49" s="1">
-        <f t="shared" si="18"/>
-        <v>39.689999999999962</v>
+        <f t="shared" si="19"/>
+        <v>216.09000000000009</v>
       </c>
       <c r="N49" s="1">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("countunique(A$4:A$33)"),3)</f>
         <v>3</v>
       </c>
       <c r="O49" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F50" s="1">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="H50" s="1">
         <f t="shared" si="14"/>
         <v>93.3</v>
       </c>
       <c r="I50" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>101.7</v>
       </c>
       <c r="J50" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-8.4000000000000057</v>
       </c>
       <c r="K50" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>70.560000000000102</v>
       </c>
       <c r="L50" s="1">
-        <f t="shared" si="17"/>
-        <v>4.7000000000000028</v>
+        <f t="shared" si="18"/>
+        <v>19.700000000000003</v>
       </c>
       <c r="M50" s="1">
-        <f t="shared" si="18"/>
-        <v>22.090000000000028</v>
+        <f t="shared" si="19"/>
+        <v>388.09000000000009</v>
       </c>
       <c r="N50" s="1">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("countunique(A$4:A$33)"),3)</f>
         <v>3</v>
       </c>
       <c r="O50" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F51" s="1">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="H51" s="1">
         <f t="shared" si="14"/>
         <v>93.3</v>
       </c>
       <c r="I51" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>101.7</v>
       </c>
       <c r="J51" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-8.4000000000000057</v>
       </c>
       <c r="K51" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>70.560000000000102</v>
       </c>
       <c r="L51" s="1">
-        <f t="shared" si="17"/>
-        <v>14.700000000000003</v>
+        <f t="shared" si="18"/>
+        <v>2.7000000000000028</v>
       </c>
       <c r="M51" s="1">
-        <f t="shared" si="18"/>
-        <v>216.09000000000009</v>
+        <f t="shared" si="19"/>
+        <v>7.2900000000000151</v>
       </c>
       <c r="N51" s="1">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("countunique(A$4:A$33)"),3)</f>
         <v>3</v>
       </c>
       <c r="O51" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F52" s="1">
-        <v>113</v>
-      </c>
-      <c r="H52" s="1">
-        <f t="shared" si="14"/>
-        <v>93.3</v>
-      </c>
-      <c r="I52" s="1">
-        <f t="shared" si="20"/>
-        <v>101.7</v>
-      </c>
-      <c r="J52" s="1">
-        <f t="shared" si="15"/>
-        <v>-8.4000000000000057</v>
-      </c>
-      <c r="K52" s="1">
-        <f t="shared" si="16"/>
-        <v>70.560000000000102</v>
-      </c>
-      <c r="L52" s="1">
-        <f t="shared" si="17"/>
-        <v>19.700000000000003</v>
-      </c>
-      <c r="M52" s="1">
-        <f t="shared" si="18"/>
-        <v>388.09000000000009</v>
-      </c>
-      <c r="N52" s="1">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("countunique(A$4:A$33)"),3)</f>
+      <c r="J52" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K52" s="3">
+        <f>SUM(K12:K51)</f>
+        <v>1956.1999999999998</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M52" s="3">
+        <f>SUM(M12:M51)</f>
+        <v>4294.1000000000004</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M53" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="N53" s="3">
+        <f ca="1">AVERAGE(N12:N51)</f>
         <v>3</v>
       </c>
-      <c r="O52" s="1">
-        <f t="shared" si="19"/>
+      <c r="O53" s="3">
+        <f>AVERAGE(O12:O51)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F53" s="1">
-        <v>96</v>
-      </c>
-      <c r="H53" s="1">
-        <f t="shared" si="14"/>
-        <v>93.3</v>
-      </c>
-      <c r="I53" s="1">
-        <f t="shared" si="20"/>
-        <v>101.7</v>
-      </c>
-      <c r="J53" s="1">
-        <f t="shared" si="15"/>
-        <v>-8.4000000000000057</v>
-      </c>
-      <c r="K53" s="1">
-        <f t="shared" si="16"/>
-        <v>70.560000000000102</v>
-      </c>
-      <c r="L53" s="1">
-        <f t="shared" si="17"/>
-        <v>2.7000000000000028</v>
-      </c>
-      <c r="M53" s="1">
-        <f t="shared" si="18"/>
-        <v>7.2900000000000151</v>
-      </c>
-      <c r="N53" s="1">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("countunique(A$4:A$33)"),3)</f>
-        <v>3</v>
-      </c>
-      <c r="O53" s="1">
-        <f t="shared" si="19"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="K54" s="1">
-        <f>SUM(K12:K53)</f>
-        <v>1956.1999999999998</v>
-      </c>
-      <c r="M54" s="1">
-        <f>SUM(M12:M53)</f>
-        <v>4294.1000000000004</v>
-      </c>
-    </row>
+    <row r="54" spans="1:15" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="55" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N55" s="1">
-        <f ca="1">AVERAGE(N12:N53)</f>
-        <v>3</v>
-      </c>
-      <c r="O55" s="1">
-        <f>AVERAGE(O12:O53)</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" ht="12.75" x14ac:dyDescent="0.2"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B56" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="57" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
-        <v>35</v>
+      <c r="C57" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E57" s="1">
+        <f t="shared" ref="E57:E65" si="21">J57</f>
+        <v>1956.1999999999998</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G57" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J57" s="1">
+        <f>K52</f>
+        <v>1956.1999999999998</v>
       </c>
     </row>
     <row r="58" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B58" s="1" t="s">
+      <c r="C58" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E58" s="1">
+        <f t="shared" ca="1" si="21"/>
+        <v>2</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>38</v>
+      <c r="G58" s="1">
+        <v>1E-3</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="J58" s="1">
+        <f ca="1">N53-1</f>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C59" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E59" s="1">
-        <f t="shared" ref="E59:E67" si="21">J59</f>
-        <v>1956.1999999999998</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>978.09999999999991</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G59" s="1">
         <v>1E-3</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J59" s="1">
-        <f>K54</f>
-        <v>1956.1999999999998</v>
+        <f ca="1">J57/J58</f>
+        <v>978.09999999999991</v>
       </c>
     </row>
     <row r="60" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C60" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E60" s="1">
-        <f t="shared" ca="1" si="21"/>
-        <v>2</v>
+        <f t="shared" si="21"/>
+        <v>4294.1000000000004</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G60" s="1">
         <v>1E-3</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J60" s="1">
-        <f ca="1">N55-1</f>
-        <v>2</v>
+        <f>M52</f>
+        <v>4294.1000000000004</v>
       </c>
     </row>
     <row r="61" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C61" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E61" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>978.09999999999991</v>
+        <v>27</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G61" s="1">
         <v>1E-3</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J61" s="1">
-        <f ca="1">J59/J60</f>
-        <v>978.09999999999991</v>
+        <f ca="1">O53-N53</f>
+        <v>27</v>
       </c>
     </row>
     <row r="62" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C62" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E62" s="1">
-        <f t="shared" si="21"/>
-        <v>4294.1000000000004</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>159.04074074074074</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G62" s="1">
         <v>1E-3</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J62" s="1">
-        <f>M54</f>
-        <v>4294.1000000000004</v>
+        <f ca="1">J60/J61</f>
+        <v>159.04074074074074</v>
       </c>
     </row>
     <row r="63" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C63" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E63" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>27</v>
+        <v>6.1499965068349587</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G63" s="1">
         <v>1E-3</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J63" s="1">
-        <f ca="1">O55-N55</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+        <f ca="1">J59/J62</f>
+        <v>6.1499965068349587</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C64" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E64" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>159.04074074074074</v>
+        <v>6.2966916787415188E-3</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G64" s="1">
         <v>1E-3</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="J64" s="1">
-        <f ca="1">J62/J63</f>
-        <v>159.04074074074074</v>
-      </c>
-    </row>
-    <row r="65" spans="3:10" ht="12.75" x14ac:dyDescent="0.2">
+        <f ca="1">FDIST(J63,J58,J61)</f>
+        <v>6.2966916787415188E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="3:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C65" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E65" s="1">
-        <f t="shared" ca="1" si="21"/>
-        <v>6.1499965068349587</v>
+        <f t="shared" si="21"/>
+        <v>0.31297697710509892</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G65" s="1">
         <v>1E-3</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J65" s="1">
-        <f ca="1">J61/J64</f>
-        <v>6.1499965068349587</v>
-      </c>
-    </row>
-    <row r="66" spans="3:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="C66" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E66" s="1">
-        <f t="shared" ca="1" si="21"/>
-        <v>6.2966916787415188E-3</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G66" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J66" s="1">
-        <f ca="1">FDIST(J65,J60,J63)</f>
-        <v>6.2966916787415188E-3</v>
-      </c>
-    </row>
-    <row r="67" spans="3:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="C67" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E67" s="1">
-        <f t="shared" si="21"/>
+        <f>J57/(J57+J60)</f>
         <v>0.31297697710509892</v>
       </c>
-      <c r="F67" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G67" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="I67" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J67" s="1">
-        <f>J59/(J59+J62)</f>
-        <v>0.31297697710509892</v>
-      </c>
-    </row>
+    </row>
+    <row r="66" spans="3:10" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="67" spans="3:10" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="68" spans="3:10" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="69" spans="3:10" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="70" spans="3:10" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -3262,80 +3806,58 @@
     <row r="1018" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="1019" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="1020" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1021" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="1022" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD2 A3:G5 J3:XFD5 A6:XFD1048576">
-    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
       <formula>"Assert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="5" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="6" operator="equal">
       <formula>"Given a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
       <formula>"Specification"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="15" priority="15" operator="beginsWith" text="With Properties">
+    <cfRule type="beginsWith" dxfId="34" priority="8" operator="beginsWith" text="With Properties">
       <formula>LEFT(A1,LEN("With Properties"))="With Properties"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="14" priority="16" operator="endsWith" text=" table of">
+    <cfRule type="endsWith" dxfId="33" priority="9" operator="endsWith" text=" table of">
       <formula>RIGHT(A1,LEN(" table of"))=" table of"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="13" priority="17" operator="endsWith" text=" of">
+    <cfRule type="endsWith" dxfId="32" priority="10" operator="endsWith" text=" of">
       <formula>RIGHT(A1,LEN(" of"))=" of"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="18">
+    <cfRule type="expression" dxfId="31" priority="11">
       <formula>AND((RIGHT(A1048576, 3) = " of"), A2 = "With Properties")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="19">
+    <cfRule type="expression" dxfId="30" priority="12">
       <formula>AND(RIGHT(XFD1, 3) = " of", A2 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD2 A3:G5 J3:XFD5 A6:XFD1048576">
-    <cfRule type="notContainsBlanks" dxfId="10" priority="20">
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="notContainsBlanks" dxfId="29" priority="13">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:I5">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
-      <formula>"Assert"</formula>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
+      <formula>"PercentagePrecision"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
-      <formula>"Given a"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
-      <formula>"Specification"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="5" priority="5" operator="beginsWith" text="With Properties">
-      <formula>LEFT(H3,LEN("With Properties"))="With Properties"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="4" priority="6" operator="endsWith" text=" table of">
-      <formula>RIGHT(H3,LEN(" table of"))=" table of"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="3" priority="7" operator="endsWith" text=" of">
-      <formula>RIGHT(H3,LEN(" of"))=" of"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="8">
-      <formula>AND((RIGHT(H2, 3) = " of"), H4 = "With Properties")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="9">
-      <formula>AND(RIGHT(G3, 3) = " of", H4 = "With Properties")</formula>
+    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
+      <formula>"="</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:I5">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="10">
-      <formula>LEN(TRIM(H3))&gt;0</formula>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
+      <formula>"StringFormat"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="I1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Generate excel tests from C# and fix problems in Underscores setup
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/Anova.xlsx
+++ b/SampleTests/ExcelTests/Anova.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\SampleTests\ExcelTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CFA5DECF-1ADD-48DC-BC3D-38EC57127370}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{582E54C8-7939-4C80-A0DF-A830F3BA4BE7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,9 +106,6 @@
     <t>VariableDescription of</t>
   </si>
   <si>
-    <t>Values table of</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -163,18 +160,12 @@
     <t>Nested Property Setup</t>
   </si>
   <si>
-    <t>Table property setup (using "table of"</t>
-  </si>
-  <si>
     <t>Nested assertions</t>
   </si>
   <si>
     <t>Calculations in the assertions (which do not get overwrttien when round tripping)</t>
   </si>
   <si>
-    <t>Tables within tables (the last nested table can use the "table of" syntax, but higher up the hierarchy the "PropertyName(index) of" syntax must be used</t>
-  </si>
-  <si>
     <t>Groups list of</t>
   </si>
   <si>
@@ -185,6 +176,15 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>Values_table of</t>
+  </si>
+  <si>
+    <t>Tables within tables (the last nested table can use the "table of" syntax, but higher up the hierarchy the "list of" syntax must be used</t>
+  </si>
+  <si>
+    <t>Table property setup (using "table of")</t>
   </si>
 </sst>
 </file>
@@ -238,7 +238,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="86">
+  <dxfs count="13">
     <dxf>
       <fill>
         <patternFill>
@@ -257,601 +257,6 @@
       <fill>
         <patternFill>
           <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1252,8 +657,8 @@
   </sheetPr>
   <dimension ref="A1:O1020"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1285,7 +690,7 @@
         <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
@@ -1305,10 +710,10 @@
         <v>24</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
@@ -1316,7 +721,7 @@
         <v>25</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
@@ -1324,29 +729,29 @@
         <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C6" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D7" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
@@ -1354,18 +759,18 @@
         <v>26</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="E9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="H9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
@@ -1375,7 +780,7 @@
     </row>
     <row r="11" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="F11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>3</v>
@@ -1774,7 +1179,7 @@
     </row>
     <row r="22" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D22" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
@@ -1782,15 +1187,15 @@
         <v>26</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="E24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="25" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
@@ -1800,7 +1205,7 @@
     </row>
     <row r="26" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F26" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
@@ -2175,7 +1580,7 @@
     </row>
     <row r="37" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="D37" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
@@ -2183,15 +1588,15 @@
         <v>26</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="E39" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="40" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
@@ -2201,7 +1606,7 @@
     </row>
     <row r="41" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F41" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
@@ -2576,14 +1981,14 @@
     </row>
     <row r="52" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J52" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K52" s="3">
         <f>SUM(K12:K51)</f>
         <v>1956.1999999999998</v>
       </c>
       <c r="L52" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M52" s="3">
         <f>SUM(M12:M51)</f>
@@ -2592,13 +1997,13 @@
     </row>
     <row r="53" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M53" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="N53" s="3">
         <f ca="1">AVERAGE(N12:N51)</f>
@@ -2612,15 +2017,15 @@
     <row r="54" spans="1:15" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="55" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B56" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>11</v>
@@ -2631,14 +2036,14 @@
         <v>12</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E57" s="1">
         <f t="shared" ref="E57:E65" si="21">J57</f>
         <v>1956.1999999999998</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G57" s="1">
         <v>1E-3</v>
@@ -2656,14 +2061,14 @@
         <v>13</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E58" s="1">
         <f t="shared" ca="1" si="21"/>
         <v>2</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G58" s="1">
         <v>1E-3</v>
@@ -2681,14 +2086,14 @@
         <v>14</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E59" s="1">
         <f t="shared" ca="1" si="21"/>
         <v>978.09999999999991</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G59" s="1">
         <v>1E-3</v>
@@ -2706,14 +2111,14 @@
         <v>15</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E60" s="1">
         <f t="shared" si="21"/>
         <v>4294.1000000000004</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G60" s="1">
         <v>1E-3</v>
@@ -2731,14 +2136,14 @@
         <v>16</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E61" s="1">
         <f t="shared" ca="1" si="21"/>
         <v>27</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G61" s="1">
         <v>1E-3</v>
@@ -2756,14 +2161,14 @@
         <v>17</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E62" s="1">
         <f t="shared" ca="1" si="21"/>
         <v>159.04074074074074</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G62" s="1">
         <v>1E-3</v>
@@ -2781,14 +2186,14 @@
         <v>18</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E63" s="1">
         <f t="shared" ca="1" si="21"/>
         <v>6.1499965068349587</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G63" s="1">
         <v>1E-3</v>
@@ -2803,17 +2208,17 @@
     </row>
     <row r="64" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C64" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E64" s="1">
         <f t="shared" ca="1" si="21"/>
         <v>6.2966916787415188E-3</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G64" s="1">
         <v>1E-3</v>
@@ -2828,17 +2233,17 @@
     </row>
     <row r="65" spans="3:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C65" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E65" s="1">
         <f t="shared" si="21"/>
         <v>0.31297697710509892</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G65" s="1">
         <v>1E-3</v>
@@ -3808,49 +3213,49 @@
     <row r="1020" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>"Assert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>"Given a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"Specification"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="34" priority="8" operator="beginsWith" text="With Properties">
+    <cfRule type="beginsWith" dxfId="8" priority="8" operator="beginsWith" text="With Properties">
       <formula>LEFT(A1,LEN("With Properties"))="With Properties"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="33" priority="9" operator="endsWith" text=" table of">
+    <cfRule type="endsWith" dxfId="7" priority="9" operator="endsWith" text=" table of">
       <formula>RIGHT(A1,LEN(" table of"))=" table of"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="32" priority="10" operator="endsWith" text=" of">
+    <cfRule type="endsWith" dxfId="6" priority="10" operator="endsWith" text=" of">
       <formula>RIGHT(A1,LEN(" of"))=" of"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="11">
+    <cfRule type="expression" dxfId="5" priority="11">
       <formula>AND((RIGHT(A1048576, 3) = " of"), A2 = "With Properties")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="12">
+    <cfRule type="expression" dxfId="4" priority="12">
       <formula>AND(RIGHT(XFD1, 3) = " of", A2 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="notContainsBlanks" dxfId="29" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="13">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"PercentagePrecision"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"="</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"StringFormat"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Don't namespace framework supplied specification specific setup classes
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/Anova.xlsx
+++ b/SampleTests/ExcelTests/Anova.xlsx
@@ -770,7 +770,7 @@
       </x:c>
       <x:c r="F9" s="1" t="inlineStr">
         <x:is>
-          <x:t>CustomerTestsExcel.ClassGeneration.Float</x:t>
+          <x:t>Float</x:t>
         </x:is>
       </x:c>
       <x:c r="H9" s="2" t="s">
@@ -1200,7 +1200,7 @@
       </x:c>
       <x:c r="F24" s="1" t="inlineStr">
         <x:is>
-          <x:t>CustomerTestsExcel.ClassGeneration.Float</x:t>
+          <x:t>Float</x:t>
         </x:is>
       </x:c>
     </x:row>
@@ -1603,7 +1603,7 @@
       </x:c>
       <x:c r="F39" s="1" t="inlineStr">
         <x:is>
-          <x:t>CustomerTestsExcel.ClassGeneration.Float</x:t>
+          <x:t>Float</x:t>
         </x:is>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
Support lists of floats when generating specification specific classes
This allows me to remove the custom SpecificationSpecificGroup class,
which is now generated
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/Anova.xlsx
+++ b/SampleTests/ExcelTests/Anova.xlsx
@@ -765,8 +765,10 @@
       </x:c>
     </x:row>
     <x:row r="9" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
-      <x:c r="E9" s="1" t="s">
-        <x:v>52</x:v>
+      <x:c r="E9" s="1" t="inlineStr">
+        <x:is>
+          <x:t>Floats_table of</x:t>
+        </x:is>
       </x:c>
       <x:c r="F9" s="1" t="inlineStr">
         <x:is>
@@ -783,8 +785,10 @@
       </x:c>
     </x:row>
     <x:row r="11" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
-      <x:c r="F11" s="1" t="s">
-        <x:v>29</x:v>
+      <x:c r="F11" s="1" t="inlineStr">
+        <x:is>
+          <x:t>Float of</x:t>
+        </x:is>
       </x:c>
       <x:c r="H11" s="1" t="s">
         <x:v>3</x:v>
@@ -1195,8 +1199,10 @@
       </x:c>
     </x:row>
     <x:row r="24" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
-      <x:c r="E24" s="1" t="s">
-        <x:v>52</x:v>
+      <x:c r="E24" s="1" t="inlineStr">
+        <x:is>
+          <x:t>Floats_table of</x:t>
+        </x:is>
       </x:c>
       <x:c r="F24" s="1" t="inlineStr">
         <x:is>
@@ -1210,8 +1216,10 @@
       </x:c>
     </x:row>
     <x:row r="26" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
-      <x:c r="F26" s="1" t="s">
-        <x:v>29</x:v>
+      <x:c r="F26" s="1" t="inlineStr">
+        <x:is>
+          <x:t>Float of</x:t>
+        </x:is>
       </x:c>
     </x:row>
     <x:row r="27" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
@@ -1598,8 +1606,10 @@
       </x:c>
     </x:row>
     <x:row r="39" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
-      <x:c r="E39" s="1" t="s">
-        <x:v>52</x:v>
+      <x:c r="E39" s="1" t="inlineStr">
+        <x:is>
+          <x:t>Floats_table of</x:t>
+        </x:is>
       </x:c>
       <x:c r="F39" s="1" t="inlineStr">
         <x:is>
@@ -1613,8 +1623,10 @@
       </x:c>
     </x:row>
     <x:row r="41" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
-      <x:c r="F41" s="1" t="s">
-        <x:v>29</x:v>
+      <x:c r="F41" s="1" t="inlineStr">
+        <x:is>
+          <x:t>Float of</x:t>
+        </x:is>
       </x:c>
     </x:row>
     <x:row r="42" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Move remaining i/o to testprojectcreator wrapper
The fact that the stream has to remain open to read the excel files
is a major annoyance.

Can now refactor the classes internally a little bit
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/Anova.xlsx
+++ b/SampleTests/ExcelTests/Anova.xlsx
@@ -767,7 +767,7 @@
     <x:row r="9" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <x:c r="E9" s="1" t="inlineStr">
         <x:is>
-          <x:t>Floats_table of</x:t>
+          <x:t>Floats table of</x:t>
         </x:is>
       </x:c>
       <x:c r="F9" s="1" t="inlineStr">
@@ -1201,7 +1201,7 @@
     <x:row r="24" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <x:c r="E24" s="1" t="inlineStr">
         <x:is>
-          <x:t>Floats_table of</x:t>
+          <x:t>Floats table of</x:t>
         </x:is>
       </x:c>
       <x:c r="F24" s="1" t="inlineStr">
@@ -1608,7 +1608,7 @@
     <x:row r="39" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
       <x:c r="E39" s="1" t="inlineStr">
         <x:is>
-          <x:t>Floats_table of</x:t>
+          <x:t>Floats table of</x:t>
         </x:is>
       </x:c>
       <x:c r="F39" s="1" t="inlineStr">

</xml_diff>

<commit_message>
Add documentation for Excel syntax
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/Anova.xlsx
+++ b/SampleTests/ExcelTests/Anova.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\SampleTests\ExcelTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642A13C8-0558-4ECE-8BC6-8C310D6DDF81}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3BA900-CC72-4011-B006-BB11E4032ADD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="55">
   <si>
     <t>Example from:</t>
   </si>
@@ -246,7 +246,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="13">
     <dxf>
       <fill>
         <patternFill>
@@ -317,109 +317,6 @@
       <fill>
         <patternFill>
           <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -768,9 +665,7 @@
   </sheetPr>
   <dimension ref="A1:O1020"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -781,13 +676,13 @@
     <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="24.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23" style="1" customWidth="1"/>
-    <col min="12" max="12" width="28.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="1"/>
-    <col min="14" max="14" width="36.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" style="1" customWidth="1"/>
     <col min="15" max="15" width="14.42578125" style="1"/>
     <col min="16" max="16" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="14.42578125" style="1"/>
@@ -1314,9 +1209,33 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="4:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="F26" s="1" t="s">
         <v>53</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="4:15" ht="12.75" x14ac:dyDescent="0.2">
@@ -3324,49 +3243,49 @@
     <row r="1020" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>"Given a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"Specification"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="22" priority="8" operator="beginsWith" text="With Properties">
+    <cfRule type="beginsWith" dxfId="8" priority="8" operator="beginsWith" text="With Properties">
       <formula>LEFT(A1,LEN("With Properties"))="With Properties"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="21" priority="9" operator="endsWith" text=" table of">
+    <cfRule type="endsWith" dxfId="7" priority="9" operator="endsWith" text=" table of">
       <formula>RIGHT(A1,LEN(" table of"))=" table of"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="20" priority="10" operator="endsWith" text=" of">
+    <cfRule type="endsWith" dxfId="6" priority="10" operator="endsWith" text=" of">
       <formula>RIGHT(A1,LEN(" of"))=" of"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="11">
+    <cfRule type="expression" dxfId="5" priority="11">
       <formula>AND((RIGHT(A1048576, 3) = " of"), A2 = "With Properties")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="12">
+    <cfRule type="expression" dxfId="4" priority="12">
       <formula>AND(RIGHT(XFD1, 3) = " of", A2 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="notContainsBlanks" dxfId="17" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="13">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"PercentagePrecision"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"="</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"StringFormat"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>